<commit_message>
examples and overview doc
</commit_message>
<xml_diff>
--- a/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
+++ b/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7C81442-ECB1-4657-8AE6-EF0812A4B05B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBF0EABF-23E3-4298-9048-62BBF4AC57FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="24315" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="169">
   <si>
     <t xml:space="preserve">Latest Version History </t>
   </si>
@@ -538,12 +538,30 @@
   <si>
     <t>Cert must be set up with permissions to use enhanced reporting  functions.</t>
   </si>
+  <si>
+    <t>Invalid month</t>
+  </si>
+  <si>
+    <t>MonthlyReportRequest</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Unable to request a Monthly ERR Report for current or future Months.  A Monthly ERR Report will only be available once a month has ended</t>
+  </si>
+  <si>
+    <t>Report available for the current year and up to the previous 4 years. The earliest year available is ${minTaxYear} </t>
+  </si>
+  <si>
+    <t>Invalid look up period</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,6 +1031,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1020,9 +1041,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -21724,11 +21742,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B8:E67"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView zoomScale="70" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="13.28515625" style="12" customWidth="1"/>
@@ -21739,7 +21757,7 @@
     <col min="7" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="71" t="s">
         <v>0</v>
       </c>
@@ -21747,13 +21765,13 @@
       <c r="D8" s="71"/>
       <c r="E8" s="71"/>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="71"/>
       <c r="C9" s="71"/>
       <c r="D9" s="71"/>
       <c r="E9" s="71"/>
     </row>
-    <row r="11" spans="2:5" ht="30">
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>1</v>
       </c>
@@ -21764,7 +21782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="23">
         <v>0.1</v>
       </c>
@@ -21773,277 +21791,277 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="39"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
       <c r="D14" s="37"/>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="11"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="38"/>
       <c r="C19" s="9"/>
       <c r="D19" s="37"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
       <c r="C25" s="9"/>
       <c r="D25" s="37"/>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="11"/>
       <c r="C31" s="37"/>
       <c r="D31" s="9"/>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
       <c r="D32" s="43"/>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="44"/>
       <c r="C33" s="46"/>
       <c r="D33" s="45"/>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="44"/>
       <c r="C34" s="44"/>
       <c r="D34" s="45"/>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
       <c r="D35" s="45"/>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="44"/>
       <c r="C36" s="44"/>
       <c r="D36" s="45"/>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="44"/>
       <c r="C37" s="47"/>
       <c r="D37" s="45"/>
     </row>
-    <row r="38" spans="2:4" ht="15.75">
+    <row r="38" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="44"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="44"/>
       <c r="C39" s="44"/>
       <c r="D39" s="48"/>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="44"/>
       <c r="C40" s="44"/>
       <c r="D40" s="45"/>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="44"/>
       <c r="C41" s="44"/>
       <c r="D41" s="45"/>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="44"/>
       <c r="C42" s="53"/>
       <c r="D42" s="45"/>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="44"/>
       <c r="C43" s="44"/>
       <c r="D43" s="45"/>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="44"/>
       <c r="C44" s="44"/>
       <c r="D44" s="48"/>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="44"/>
       <c r="C45" s="56"/>
       <c r="D45" s="45"/>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="44"/>
       <c r="C46" s="44"/>
       <c r="D46" s="45"/>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="44"/>
       <c r="C47" s="44"/>
       <c r="D47" s="45"/>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="57"/>
       <c r="C48" s="57"/>
       <c r="D48" s="43"/>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="44"/>
       <c r="C49" s="44"/>
       <c r="D49" s="45"/>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="44"/>
       <c r="C50" s="44"/>
       <c r="D50" s="45"/>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="44"/>
       <c r="C51" s="44"/>
       <c r="D51" s="45"/>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="44"/>
       <c r="C52" s="44"/>
       <c r="D52" s="48"/>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="44"/>
       <c r="C53" s="44"/>
       <c r="D53" s="45"/>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
       <c r="D54" s="45"/>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="44"/>
       <c r="C55" s="44"/>
       <c r="D55" s="45"/>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="44"/>
       <c r="C56" s="44"/>
       <c r="D56" s="45"/>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="44"/>
       <c r="C57" s="44"/>
       <c r="D57" s="45"/>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="44"/>
       <c r="C58" s="44"/>
       <c r="D58" s="45"/>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="44"/>
       <c r="C59" s="44"/>
       <c r="D59" s="45"/>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="44"/>
       <c r="C60" s="44"/>
       <c r="D60" s="45"/>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="44"/>
       <c r="C61" s="44"/>
       <c r="D61" s="45"/>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="44"/>
       <c r="C62" s="44"/>
       <c r="D62" s="45"/>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="44"/>
       <c r="C63" s="44"/>
       <c r="D63" s="45"/>
     </row>
-    <row r="64" spans="2:4">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="44"/>
       <c r="C64" s="44"/>
       <c r="D64" s="48"/>
     </row>
-    <row r="65" spans="2:4">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="44"/>
       <c r="C65" s="44"/>
       <c r="D65" s="45"/>
     </row>
-    <row r="66" spans="2:4">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="44"/>
       <c r="C66" s="44"/>
       <c r="D66" s="45"/>
     </row>
-    <row r="67" spans="2:4">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="44"/>
       <c r="C67" s="44"/>
       <c r="D67" s="48"/>
@@ -22063,13 +22081,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM338"/>
+  <dimension ref="A1:BM339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{4B0FFF15-58BE-5FF3-BF7D-C0BFE47F2011}">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="6" customWidth="1"/>
@@ -22086,7 +22104,7 @@
     <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="47.25">
+    <row r="1" spans="1:65" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>5</v>
       </c>
@@ -22134,7 +22152,7 @@
       </c>
       <c r="P1" s="14"/>
     </row>
-    <row r="2" spans="1:65" ht="18.75" customHeight="1">
+    <row r="2" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
         <v>20</v>
       </c>
@@ -22151,30 +22169,30 @@
       <c r="L2" s="73"/>
       <c r="M2" s="73"/>
       <c r="N2" s="73"/>
-      <c r="O2" s="77"/>
+      <c r="O2" s="74"/>
       <c r="P2" s="15"/>
     </row>
-    <row r="3" spans="1:65" ht="15.75" customHeight="1">
-      <c r="A3" s="74" t="s">
+    <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="76"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="77"/>
       <c r="P3" s="15"/>
     </row>
-    <row r="4" spans="1:65" outlineLevel="1">
+    <row r="4" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54">
         <v>146</v>
       </c>
@@ -22222,7 +22240,7 @@
       </c>
       <c r="P4" s="15"/>
     </row>
-    <row r="5" spans="1:65" ht="63" outlineLevel="1">
+    <row r="5" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -22270,7 +22288,7 @@
       </c>
       <c r="P5" s="15"/>
     </row>
-    <row r="6" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="6" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -22318,7 +22336,7 @@
       </c>
       <c r="P6" s="15"/>
     </row>
-    <row r="7" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="7" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -22365,7 +22383,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="8" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -22412,7 +22430,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="9" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>77</v>
       </c>
@@ -22508,7 +22526,7 @@
       <c r="BL9" s="16"/>
       <c r="BM9" s="16"/>
     </row>
-    <row r="10" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="10" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>116</v>
       </c>
@@ -22555,7 +22573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:65" outlineLevel="1">
+    <row r="11" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -22602,7 +22620,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:65" outlineLevel="1">
+    <row r="12" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -22649,7 +22667,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="13" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -22696,7 +22714,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="14" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -22743,7 +22761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:65" ht="63" outlineLevel="1">
+    <row r="15" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>10</v>
       </c>
@@ -22790,7 +22808,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="16" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>100</v>
       </c>
@@ -22837,7 +22855,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="17" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>17</v>
       </c>
@@ -22884,7 +22902,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="47.25" outlineLevel="1">
+    <row r="18" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>144</v>
       </c>
@@ -22932,27 +22950,27 @@
       </c>
       <c r="P18" s="27"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A19" s="74" t="s">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="76"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="76"/>
+      <c r="O19" s="77"/>
       <c r="P19" s="15"/>
     </row>
-    <row r="20" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="20" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>152</v>
       </c>
@@ -23000,7 +23018,7 @@
       </c>
       <c r="P20" s="15"/>
     </row>
-    <row r="21" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="21" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>153</v>
       </c>
@@ -23048,7 +23066,7 @@
       </c>
       <c r="P21" s="15"/>
     </row>
-    <row r="22" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="22" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>126</v>
       </c>
@@ -23095,7 +23113,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="23" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>19</v>
       </c>
@@ -23142,7 +23160,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="24" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>97</v>
       </c>
@@ -23189,7 +23207,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="25" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>143</v>
       </c>
@@ -23237,7 +23255,7 @@
       </c>
       <c r="P25" s="27"/>
     </row>
-    <row r="26" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="26" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>20</v>
       </c>
@@ -23284,7 +23302,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="63" outlineLevel="1">
+    <row r="27" spans="1:16" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>22</v>
       </c>
@@ -23331,7 +23349,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="28" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>23</v>
       </c>
@@ -23378,7 +23396,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="29" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>31</v>
       </c>
@@ -23425,7 +23443,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="30" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <v>134</v>
       </c>
@@ -23472,7 +23490,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="31" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>32</v>
       </c>
@@ -23519,7 +23537,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="47.25" outlineLevel="1">
+    <row r="32" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>42</v>
       </c>
@@ -23566,7 +23584,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="33" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>43</v>
       </c>
@@ -23613,7 +23631,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="34" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>51</v>
       </c>
@@ -23660,7 +23678,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="35" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>160</v>
       </c>
@@ -23707,7 +23725,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="36" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>161</v>
       </c>
@@ -23754,7 +23772,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="37" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>162</v>
       </c>
@@ -23801,7 +23819,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="38" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>168</v>
       </c>
@@ -23848,7 +23866,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="39" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>163</v>
       </c>
@@ -23895,7 +23913,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="40" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>164</v>
       </c>
@@ -23942,7 +23960,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="47.25" outlineLevel="1">
+    <row r="41" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>165</v>
       </c>
@@ -23989,7 +24007,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="42" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>166</v>
       </c>
@@ -24036,7 +24054,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="43" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>167</v>
       </c>
@@ -24083,7 +24101,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="18.75" customHeight="1">
+    <row r="44" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="72" t="s">
         <v>127</v>
       </c>
@@ -24100,30 +24118,30 @@
       <c r="L44" s="73"/>
       <c r="M44" s="73"/>
       <c r="N44" s="73"/>
-      <c r="O44" s="77"/>
+      <c r="O44" s="74"/>
       <c r="P44" s="15"/>
     </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A45" s="74" t="s">
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="75"/>
-      <c r="I45" s="75"/>
-      <c r="J45" s="75"/>
-      <c r="K45" s="75"/>
-      <c r="L45" s="75"/>
-      <c r="M45" s="75"/>
-      <c r="N45" s="75"/>
-      <c r="O45" s="76"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="77"/>
       <c r="P45" s="15"/>
     </row>
-    <row r="46" spans="1:16" ht="47.25" outlineLevel="1">
+    <row r="46" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="54">
         <v>148</v>
       </c>
@@ -24171,7 +24189,7 @@
       </c>
       <c r="P46" s="15"/>
     </row>
-    <row r="47" spans="1:16" ht="31.5" outlineLevel="1">
+    <row r="47" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="54">
         <v>146</v>
       </c>
@@ -24219,7 +24237,7 @@
       </c>
       <c r="P47" s="15"/>
     </row>
-    <row r="48" spans="1:16" ht="63" outlineLevel="1">
+    <row r="48" spans="1:16" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>52</v>
       </c>
@@ -24267,7 +24285,7 @@
       </c>
       <c r="P48" s="15"/>
     </row>
-    <row r="49" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="49" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>53</v>
       </c>
@@ -24315,7 +24333,7 @@
       </c>
       <c r="P49" s="15"/>
     </row>
-    <row r="50" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="50" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>55</v>
       </c>
@@ -24362,7 +24380,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:65" ht="63" outlineLevel="1">
+    <row r="51" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>56</v>
       </c>
@@ -24409,7 +24427,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="52" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>77</v>
       </c>
@@ -24505,7 +24523,7 @@
       <c r="BL52" s="16"/>
       <c r="BM52" s="16"/>
     </row>
-    <row r="53" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="53" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>117</v>
       </c>
@@ -24552,7 +24570,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="54" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>57</v>
       </c>
@@ -24599,7 +24617,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="55" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>58</v>
       </c>
@@ -24646,7 +24664,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="56" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>59</v>
       </c>
@@ -24693,7 +24711,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="57" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>60</v>
       </c>
@@ -24740,7 +24758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="58" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>61</v>
       </c>
@@ -24787,7 +24805,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:65" ht="18.75" customHeight="1">
+    <row r="59" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="72" t="s">
         <v>138</v>
       </c>
@@ -24804,30 +24822,30 @@
       <c r="L59" s="73"/>
       <c r="M59" s="73"/>
       <c r="N59" s="73"/>
-      <c r="O59" s="77"/>
+      <c r="O59" s="74"/>
       <c r="P59" s="15"/>
     </row>
-    <row r="60" spans="1:65" ht="15.75" customHeight="1">
-      <c r="A60" s="74" t="s">
+    <row r="60" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B60" s="75"/>
-      <c r="C60" s="75"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="75"/>
-      <c r="I60" s="75"/>
-      <c r="J60" s="75"/>
-      <c r="K60" s="75"/>
-      <c r="L60" s="75"/>
-      <c r="M60" s="75"/>
-      <c r="N60" s="75"/>
-      <c r="O60" s="76"/>
+      <c r="B60" s="76"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="76"/>
+      <c r="M60" s="76"/>
+      <c r="N60" s="76"/>
+      <c r="O60" s="77"/>
       <c r="P60" s="15"/>
     </row>
-    <row r="61" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="61" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="54">
         <v>148</v>
       </c>
@@ -24875,7 +24893,7 @@
       </c>
       <c r="P61" s="15"/>
     </row>
-    <row r="62" spans="1:65" outlineLevel="1">
+    <row r="62" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="54">
         <v>146</v>
       </c>
@@ -24923,7 +24941,7 @@
       </c>
       <c r="P62" s="15"/>
     </row>
-    <row r="63" spans="1:65" ht="63" outlineLevel="1">
+    <row r="63" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -24971,7 +24989,7 @@
       </c>
       <c r="P63" s="15"/>
     </row>
-    <row r="64" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="64" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -25019,7 +25037,7 @@
       </c>
       <c r="P64" s="15"/>
     </row>
-    <row r="65" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="65" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>65</v>
       </c>
@@ -25066,7 +25084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:65" ht="63" outlineLevel="1">
+    <row r="66" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>66</v>
       </c>
@@ -25113,7 +25131,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="67" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>77</v>
       </c>
@@ -25209,7 +25227,7 @@
       <c r="BL67" s="16"/>
       <c r="BM67" s="16"/>
     </row>
-    <row r="68" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="68" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>118</v>
       </c>
@@ -25256,7 +25274,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="69" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>67</v>
       </c>
@@ -25303,7 +25321,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="70" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>68</v>
       </c>
@@ -25350,7 +25368,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="71" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>69</v>
       </c>
@@ -25397,7 +25415,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="72" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>70</v>
       </c>
@@ -25444,7 +25462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="73" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>71</v>
       </c>
@@ -25491,7 +25509,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1">
+    <row r="74" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="72" t="s">
         <v>144</v>
       </c>
@@ -25560,24 +25578,24 @@
       <c r="BL74" s="15"/>
       <c r="BM74" s="15"/>
     </row>
-    <row r="75" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A75" s="74" t="s">
+    <row r="75" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B75" s="75"/>
-      <c r="C75" s="75"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="75"/>
-      <c r="J75" s="75"/>
-      <c r="K75" s="75"/>
-      <c r="L75" s="75"/>
-      <c r="M75" s="75"/>
-      <c r="N75" s="75"/>
-      <c r="O75" s="75"/>
+      <c r="B75" s="76"/>
+      <c r="C75" s="76"/>
+      <c r="D75" s="76"/>
+      <c r="E75" s="76"/>
+      <c r="F75" s="76"/>
+      <c r="G75" s="76"/>
+      <c r="H75" s="76"/>
+      <c r="I75" s="76"/>
+      <c r="J75" s="76"/>
+      <c r="K75" s="76"/>
+      <c r="L75" s="76"/>
+      <c r="M75" s="76"/>
+      <c r="N75" s="76"/>
+      <c r="O75" s="76"/>
       <c r="P75" s="15"/>
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
@@ -25629,7 +25647,7 @@
       <c r="BL75" s="15"/>
       <c r="BM75" s="15"/>
     </row>
-    <row r="76" spans="1:65" s="6" customFormat="1" ht="40.700000000000003" customHeight="1" outlineLevel="1">
+    <row r="76" spans="1:65" s="6" customFormat="1" ht="40.700000000000003" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="54">
         <v>146</v>
       </c>
@@ -25726,7 +25744,7 @@
       <c r="BL76" s="15"/>
       <c r="BM76" s="15"/>
     </row>
-    <row r="77" spans="1:65" s="6" customFormat="1" ht="63" outlineLevel="1">
+    <row r="77" spans="1:65" s="6" customFormat="1" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>72</v>
       </c>
@@ -25823,7 +25841,7 @@
       <c r="BL77" s="15"/>
       <c r="BM77" s="15"/>
     </row>
-    <row r="78" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1">
+    <row r="78" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>73</v>
       </c>
@@ -25920,7 +25938,7 @@
       <c r="BL78" s="15"/>
       <c r="BM78" s="15"/>
     </row>
-    <row r="79" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="79" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>75</v>
       </c>
@@ -26016,7 +26034,7 @@
       <c r="BL79" s="16"/>
       <c r="BM79" s="16"/>
     </row>
-    <row r="80" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="80" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>76</v>
       </c>
@@ -26112,7 +26130,7 @@
       <c r="BL80" s="16"/>
       <c r="BM80" s="16"/>
     </row>
-    <row r="81" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="81" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>77</v>
       </c>
@@ -26208,7 +26226,7 @@
       <c r="BL81" s="16"/>
       <c r="BM81" s="16"/>
     </row>
-    <row r="82" spans="1:65" ht="47.25" outlineLevel="1">
+    <row r="82" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>119</v>
       </c>
@@ -26304,7 +26322,7 @@
       <c r="BL82" s="16"/>
       <c r="BM82" s="16"/>
     </row>
-    <row r="83" spans="1:65" outlineLevel="1">
+    <row r="83" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>78</v>
       </c>
@@ -26400,7 +26418,7 @@
       <c r="BL83" s="16"/>
       <c r="BM83" s="16"/>
     </row>
-    <row r="84" spans="1:65" outlineLevel="1">
+    <row r="84" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>79</v>
       </c>
@@ -26496,7 +26514,7 @@
       <c r="BL84" s="16"/>
       <c r="BM84" s="16"/>
     </row>
-    <row r="85" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="85" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>80</v>
       </c>
@@ -26592,7 +26610,7 @@
       <c r="BL85" s="16"/>
       <c r="BM85" s="16"/>
     </row>
-    <row r="86" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="86" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>81</v>
       </c>
@@ -26688,7 +26706,7 @@
       <c r="BL86" s="16"/>
       <c r="BM86" s="16"/>
     </row>
-    <row r="87" spans="1:65" s="6" customFormat="1" outlineLevel="1">
+    <row r="87" spans="1:65" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20">
         <v>169</v>
       </c>
@@ -26785,7 +26803,7 @@
       <c r="BL87" s="15"/>
       <c r="BM87" s="15"/>
     </row>
-    <row r="88" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1">
+    <row r="88" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="40">
         <v>156</v>
       </c>
@@ -26882,7 +26900,7 @@
       <c r="BL88" s="15"/>
       <c r="BM88" s="15"/>
     </row>
-    <row r="89" spans="1:65" ht="31.5" outlineLevel="1">
+    <row r="89" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>168</v>
       </c>
@@ -26929,7 +26947,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:65" ht="31.5">
+    <row r="90" spans="1:65" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="20">
         <v>145</v>
       </c>
@@ -26976,7 +26994,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1">
+    <row r="91" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="72" t="s">
         <v>158</v>
       </c>
@@ -27045,26 +27063,26 @@
       <c r="BL91" s="15"/>
       <c r="BM91" s="15"/>
     </row>
-    <row r="92" spans="1:65" ht="15.75" customHeight="1">
-      <c r="A92" s="74" t="s">
+    <row r="92" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B92" s="75"/>
-      <c r="C92" s="75"/>
-      <c r="D92" s="75"/>
-      <c r="E92" s="75"/>
-      <c r="F92" s="75"/>
-      <c r="G92" s="75"/>
-      <c r="H92" s="75"/>
-      <c r="I92" s="75"/>
-      <c r="J92" s="75"/>
-      <c r="K92" s="75"/>
-      <c r="L92" s="75"/>
-      <c r="M92" s="75"/>
-      <c r="N92" s="75"/>
-      <c r="O92" s="75"/>
-    </row>
-    <row r="93" spans="1:65">
+      <c r="B92" s="76"/>
+      <c r="C92" s="76"/>
+      <c r="D92" s="76"/>
+      <c r="E92" s="76"/>
+      <c r="F92" s="76"/>
+      <c r="G92" s="76"/>
+      <c r="H92" s="76"/>
+      <c r="I92" s="76"/>
+      <c r="J92" s="76"/>
+      <c r="K92" s="76"/>
+      <c r="L92" s="76"/>
+      <c r="M92" s="76"/>
+      <c r="N92" s="76"/>
+      <c r="O92" s="76"/>
+    </row>
+    <row r="93" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A93" s="54">
         <v>146</v>
       </c>
@@ -27111,7 +27129,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:65" ht="63">
+    <row r="94" spans="1:65" ht="63" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>102</v>
       </c>
@@ -27158,7 +27176,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:65" ht="31.5">
+    <row r="95" spans="1:65" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>103</v>
       </c>
@@ -27205,7 +27223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:65" ht="47.25">
+    <row r="96" spans="1:65" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>105</v>
       </c>
@@ -27252,7 +27270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="47.25">
+    <row r="97" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>106</v>
       </c>
@@ -27299,7 +27317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="47.25">
+    <row r="98" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>121</v>
       </c>
@@ -27346,7 +27364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>107</v>
       </c>
@@ -27393,7 +27411,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>108</v>
       </c>
@@ -27440,7 +27458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="31.5">
+    <row r="101" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>109</v>
       </c>
@@ -27487,7 +27505,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="47.25">
+    <row r="102" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>110</v>
       </c>
@@ -27534,7 +27552,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="31.5">
+    <row r="103" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>111</v>
       </c>
@@ -27581,7 +27599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="31.5" outlineLevel="1">
+    <row r="104" spans="1:15" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>17</v>
       </c>
@@ -27622,47 +27640,107 @@
         <v>61</v>
       </c>
       <c r="N104" s="25" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="O104" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
-      <c r="A105" s="14"/>
-      <c r="B105" s="15"/>
-      <c r="C105" s="63"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="30"/>
-      <c r="H105" s="30"/>
-      <c r="I105" s="30"/>
-      <c r="J105" s="14"/>
-      <c r="K105" s="14"/>
-      <c r="L105" s="14"/>
-      <c r="M105" s="15"/>
-      <c r="N105" s="15"/>
-      <c r="O105" s="15"/>
-    </row>
-    <row r="106" spans="1:15">
-      <c r="A106" s="14"/>
-      <c r="B106" s="15"/>
-      <c r="C106" s="63"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="30"/>
-      <c r="H106" s="30"/>
-      <c r="I106" s="30"/>
-      <c r="J106" s="14"/>
-      <c r="K106" s="14"/>
-      <c r="L106" s="14"/>
-      <c r="M106" s="15"/>
-      <c r="N106" s="15"/>
-      <c r="O106" s="15"/>
-    </row>
-    <row r="107" spans="1:15">
+    <row r="105" spans="1:15" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>112</v>
+      </c>
+      <c r="B105" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C105" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D105" s="18">
+        <v>305</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G105" s="29">
+        <v>400</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I105" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J105" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K105" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L105" s="5">
+        <v>3002</v>
+      </c>
+      <c r="M105" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="N105" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="O105" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>113</v>
+      </c>
+      <c r="B106" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D106" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F106" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" s="29">
+        <v>400</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I106" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J106" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K106" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L106" s="20">
+        <v>3003</v>
+      </c>
+      <c r="M106" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="N106" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="O106" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
       <c r="B107" s="15"/>
       <c r="C107" s="63"/>
@@ -27679,7 +27757,7 @@
       <c r="N107" s="15"/>
       <c r="O107" s="15"/>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
       <c r="B108" s="15"/>
       <c r="C108" s="63"/>
@@ -27696,7 +27774,7 @@
       <c r="N108" s="15"/>
       <c r="O108" s="15"/>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
       <c r="B109" s="15"/>
       <c r="C109" s="63"/>
@@ -27713,7 +27791,7 @@
       <c r="N109" s="15"/>
       <c r="O109" s="15"/>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="15"/>
       <c r="C110" s="63"/>
@@ -27730,7 +27808,7 @@
       <c r="N110" s="15"/>
       <c r="O110" s="15"/>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="15"/>
       <c r="C111" s="63"/>
@@ -27747,7 +27825,7 @@
       <c r="N111" s="15"/>
       <c r="O111" s="15"/>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="14"/>
       <c r="B112" s="15"/>
       <c r="C112" s="63"/>
@@ -27764,7 +27842,7 @@
       <c r="N112" s="15"/>
       <c r="O112" s="15"/>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="14"/>
       <c r="B113" s="15"/>
       <c r="C113" s="63"/>
@@ -27781,7 +27859,7 @@
       <c r="N113" s="15"/>
       <c r="O113" s="15"/>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="15"/>
       <c r="C114" s="63"/>
@@ -27798,7 +27876,7 @@
       <c r="N114" s="15"/>
       <c r="O114" s="15"/>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="15"/>
       <c r="C115" s="63"/>
@@ -27815,7 +27893,7 @@
       <c r="N115" s="15"/>
       <c r="O115" s="15"/>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
       <c r="B116" s="15"/>
       <c r="C116" s="63"/>
@@ -27832,7 +27910,7 @@
       <c r="N116" s="15"/>
       <c r="O116" s="15"/>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="15"/>
       <c r="C117" s="63"/>
@@ -27849,7 +27927,7 @@
       <c r="N117" s="15"/>
       <c r="O117" s="15"/>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="15"/>
       <c r="C118" s="63"/>
@@ -27866,7 +27944,7 @@
       <c r="N118" s="15"/>
       <c r="O118" s="15"/>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="15"/>
       <c r="C119" s="63"/>
@@ -27883,7 +27961,7 @@
       <c r="N119" s="15"/>
       <c r="O119" s="15"/>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
       <c r="B120" s="15"/>
       <c r="C120" s="63"/>
@@ -27900,7 +27978,7 @@
       <c r="N120" s="15"/>
       <c r="O120" s="15"/>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="15"/>
       <c r="C121" s="63"/>
@@ -27917,7 +27995,7 @@
       <c r="N121" s="15"/>
       <c r="O121" s="15"/>
     </row>
-    <row r="122" spans="1:15">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="15"/>
       <c r="C122" s="63"/>
@@ -27934,7 +28012,7 @@
       <c r="N122" s="15"/>
       <c r="O122" s="15"/>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="15"/>
       <c r="C123" s="63"/>
@@ -27951,7 +28029,7 @@
       <c r="N123" s="15"/>
       <c r="O123" s="15"/>
     </row>
-    <row r="124" spans="1:15">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
       <c r="B124" s="15"/>
       <c r="C124" s="63"/>
@@ -27968,7 +28046,7 @@
       <c r="N124" s="15"/>
       <c r="O124" s="15"/>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="14"/>
       <c r="B125" s="15"/>
       <c r="C125" s="63"/>
@@ -27985,7 +28063,7 @@
       <c r="N125" s="15"/>
       <c r="O125" s="15"/>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
       <c r="B126" s="15"/>
       <c r="C126" s="63"/>
@@ -28002,7 +28080,7 @@
       <c r="N126" s="15"/>
       <c r="O126" s="15"/>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="14"/>
       <c r="B127" s="15"/>
       <c r="C127" s="63"/>
@@ -28019,7 +28097,7 @@
       <c r="N127" s="15"/>
       <c r="O127" s="15"/>
     </row>
-    <row r="128" spans="1:15">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
       <c r="B128" s="15"/>
       <c r="C128" s="63"/>
@@ -28036,7 +28114,7 @@
       <c r="N128" s="15"/>
       <c r="O128" s="15"/>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="14"/>
       <c r="B129" s="15"/>
       <c r="C129" s="63"/>
@@ -28053,7 +28131,7 @@
       <c r="N129" s="15"/>
       <c r="O129" s="15"/>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="14"/>
       <c r="B130" s="15"/>
       <c r="C130" s="63"/>
@@ -28070,7 +28148,7 @@
       <c r="N130" s="15"/>
       <c r="O130" s="15"/>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="14"/>
       <c r="B131" s="15"/>
       <c r="C131" s="63"/>
@@ -28087,7 +28165,7 @@
       <c r="N131" s="15"/>
       <c r="O131" s="15"/>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="14"/>
       <c r="B132" s="15"/>
       <c r="C132" s="63"/>
@@ -28104,7 +28182,7 @@
       <c r="N132" s="15"/>
       <c r="O132" s="15"/>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="14"/>
       <c r="B133" s="15"/>
       <c r="C133" s="63"/>
@@ -28121,7 +28199,7 @@
       <c r="N133" s="15"/>
       <c r="O133" s="15"/>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="14"/>
       <c r="B134" s="15"/>
       <c r="C134" s="63"/>
@@ -28138,7 +28216,7 @@
       <c r="N134" s="15"/>
       <c r="O134" s="15"/>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="14"/>
       <c r="B135" s="15"/>
       <c r="C135" s="63"/>
@@ -28155,7 +28233,7 @@
       <c r="N135" s="15"/>
       <c r="O135" s="15"/>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="14"/>
       <c r="B136" s="15"/>
       <c r="C136" s="63"/>
@@ -28172,7 +28250,7 @@
       <c r="N136" s="15"/>
       <c r="O136" s="15"/>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="15"/>
       <c r="C137" s="63"/>
@@ -28189,7 +28267,7 @@
       <c r="N137" s="15"/>
       <c r="O137" s="15"/>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="15"/>
       <c r="C138" s="63"/>
@@ -28206,7 +28284,7 @@
       <c r="N138" s="15"/>
       <c r="O138" s="15"/>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="15"/>
       <c r="C139" s="63"/>
@@ -28223,7 +28301,7 @@
       <c r="N139" s="15"/>
       <c r="O139" s="15"/>
     </row>
-    <row r="140" spans="1:15">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
       <c r="B140" s="15"/>
       <c r="C140" s="63"/>
@@ -28240,7 +28318,7 @@
       <c r="N140" s="15"/>
       <c r="O140" s="15"/>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="15"/>
       <c r="C141" s="63"/>
@@ -28257,7 +28335,7 @@
       <c r="N141" s="15"/>
       <c r="O141" s="15"/>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="15"/>
       <c r="C142" s="63"/>
@@ -28274,7 +28352,7 @@
       <c r="N142" s="15"/>
       <c r="O142" s="15"/>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="15"/>
       <c r="C143" s="63"/>
@@ -28291,7 +28369,7 @@
       <c r="N143" s="15"/>
       <c r="O143" s="15"/>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="15"/>
       <c r="C144" s="63"/>
@@ -28308,7 +28386,7 @@
       <c r="N144" s="15"/>
       <c r="O144" s="15"/>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="14"/>
       <c r="B145" s="15"/>
       <c r="C145" s="63"/>
@@ -28325,7 +28403,7 @@
       <c r="N145" s="15"/>
       <c r="O145" s="15"/>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
       <c r="B146" s="15"/>
       <c r="C146" s="63"/>
@@ -28342,7 +28420,7 @@
       <c r="N146" s="15"/>
       <c r="O146" s="15"/>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
       <c r="B147" s="15"/>
       <c r="C147" s="63"/>
@@ -28359,7 +28437,7 @@
       <c r="N147" s="15"/>
       <c r="O147" s="15"/>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="14"/>
       <c r="B148" s="15"/>
       <c r="C148" s="63"/>
@@ -28376,7 +28454,7 @@
       <c r="N148" s="15"/>
       <c r="O148" s="15"/>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="14"/>
       <c r="B149" s="15"/>
       <c r="C149" s="63"/>
@@ -28393,7 +28471,7 @@
       <c r="N149" s="15"/>
       <c r="O149" s="15"/>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="14"/>
       <c r="B150" s="15"/>
       <c r="C150" s="63"/>
@@ -28410,7 +28488,7 @@
       <c r="N150" s="15"/>
       <c r="O150" s="15"/>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" s="14"/>
       <c r="B151" s="15"/>
       <c r="C151" s="63"/>
@@ -28427,7 +28505,7 @@
       <c r="N151" s="15"/>
       <c r="O151" s="15"/>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" s="14"/>
       <c r="B152" s="15"/>
       <c r="C152" s="63"/>
@@ -28444,7 +28522,7 @@
       <c r="N152" s="15"/>
       <c r="O152" s="15"/>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" s="14"/>
       <c r="B153" s="15"/>
       <c r="C153" s="63"/>
@@ -28461,7 +28539,7 @@
       <c r="N153" s="15"/>
       <c r="O153" s="15"/>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" s="14"/>
       <c r="B154" s="15"/>
       <c r="C154" s="63"/>
@@ -28478,7 +28556,7 @@
       <c r="N154" s="15"/>
       <c r="O154" s="15"/>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" s="14"/>
       <c r="B155" s="15"/>
       <c r="C155" s="63"/>
@@ -28495,7 +28573,7 @@
       <c r="N155" s="15"/>
       <c r="O155" s="15"/>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" s="14"/>
       <c r="B156" s="15"/>
       <c r="C156" s="63"/>
@@ -28512,7 +28590,7 @@
       <c r="N156" s="15"/>
       <c r="O156" s="15"/>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" s="14"/>
       <c r="B157" s="15"/>
       <c r="C157" s="63"/>
@@ -28529,7 +28607,7 @@
       <c r="N157" s="15"/>
       <c r="O157" s="15"/>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
       <c r="B158" s="15"/>
       <c r="C158" s="63"/>
@@ -28546,7 +28624,7 @@
       <c r="N158" s="15"/>
       <c r="O158" s="15"/>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
       <c r="B159" s="15"/>
       <c r="C159" s="63"/>
@@ -28563,7 +28641,7 @@
       <c r="N159" s="15"/>
       <c r="O159" s="15"/>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
       <c r="B160" s="15"/>
       <c r="C160" s="63"/>
@@ -28580,7 +28658,7 @@
       <c r="N160" s="15"/>
       <c r="O160" s="15"/>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="14"/>
       <c r="B161" s="15"/>
       <c r="C161" s="63"/>
@@ -28597,7 +28675,7 @@
       <c r="N161" s="15"/>
       <c r="O161" s="15"/>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="14"/>
       <c r="B162" s="15"/>
       <c r="C162" s="63"/>
@@ -28614,7 +28692,7 @@
       <c r="N162" s="15"/>
       <c r="O162" s="15"/>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" s="14"/>
       <c r="B163" s="15"/>
       <c r="C163" s="63"/>
@@ -28631,7 +28709,7 @@
       <c r="N163" s="15"/>
       <c r="O163" s="15"/>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" s="14"/>
       <c r="B164" s="15"/>
       <c r="C164" s="63"/>
@@ -28648,7 +28726,7 @@
       <c r="N164" s="15"/>
       <c r="O164" s="15"/>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" s="14"/>
       <c r="B165" s="15"/>
       <c r="C165" s="63"/>
@@ -28665,7 +28743,7 @@
       <c r="N165" s="15"/>
       <c r="O165" s="15"/>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" s="14"/>
       <c r="B166" s="15"/>
       <c r="C166" s="63"/>
@@ -28682,7 +28760,7 @@
       <c r="N166" s="15"/>
       <c r="O166" s="15"/>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" s="14"/>
       <c r="B167" s="15"/>
       <c r="C167" s="63"/>
@@ -28699,7 +28777,7 @@
       <c r="N167" s="15"/>
       <c r="O167" s="15"/>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="14"/>
       <c r="B168" s="15"/>
       <c r="C168" s="63"/>
@@ -28716,7 +28794,7 @@
       <c r="N168" s="15"/>
       <c r="O168" s="15"/>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="14"/>
       <c r="B169" s="15"/>
       <c r="C169" s="63"/>
@@ -28733,7 +28811,7 @@
       <c r="N169" s="15"/>
       <c r="O169" s="15"/>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" s="14"/>
       <c r="B170" s="15"/>
       <c r="C170" s="63"/>
@@ -28750,7 +28828,7 @@
       <c r="N170" s="15"/>
       <c r="O170" s="15"/>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" s="14"/>
       <c r="B171" s="15"/>
       <c r="C171" s="63"/>
@@ -28767,7 +28845,7 @@
       <c r="N171" s="15"/>
       <c r="O171" s="15"/>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" s="14"/>
       <c r="B172" s="15"/>
       <c r="C172" s="63"/>
@@ -28784,7 +28862,7 @@
       <c r="N172" s="15"/>
       <c r="O172" s="15"/>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" s="14"/>
       <c r="B173" s="15"/>
       <c r="C173" s="63"/>
@@ -28801,7 +28879,7 @@
       <c r="N173" s="15"/>
       <c r="O173" s="15"/>
     </row>
-    <row r="174" spans="1:15">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" s="14"/>
       <c r="B174" s="15"/>
       <c r="C174" s="63"/>
@@ -28818,7 +28896,7 @@
       <c r="N174" s="15"/>
       <c r="O174" s="15"/>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" s="14"/>
       <c r="B175" s="15"/>
       <c r="C175" s="63"/>
@@ -28835,7 +28913,7 @@
       <c r="N175" s="15"/>
       <c r="O175" s="15"/>
     </row>
-    <row r="176" spans="1:15">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" s="14"/>
       <c r="B176" s="15"/>
       <c r="C176" s="63"/>
@@ -28852,7 +28930,7 @@
       <c r="N176" s="15"/>
       <c r="O176" s="15"/>
     </row>
-    <row r="177" spans="1:15">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" s="14"/>
       <c r="B177" s="15"/>
       <c r="C177" s="63"/>
@@ -28869,7 +28947,7 @@
       <c r="N177" s="15"/>
       <c r="O177" s="15"/>
     </row>
-    <row r="178" spans="1:15">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" s="14"/>
       <c r="B178" s="15"/>
       <c r="C178" s="63"/>
@@ -28886,7 +28964,7 @@
       <c r="N178" s="15"/>
       <c r="O178" s="15"/>
     </row>
-    <row r="179" spans="1:15">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A179" s="14"/>
       <c r="B179" s="15"/>
       <c r="C179" s="63"/>
@@ -28903,7 +28981,7 @@
       <c r="N179" s="15"/>
       <c r="O179" s="15"/>
     </row>
-    <row r="180" spans="1:15">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" s="14"/>
       <c r="B180" s="15"/>
       <c r="C180" s="63"/>
@@ -28920,7 +28998,7 @@
       <c r="N180" s="15"/>
       <c r="O180" s="15"/>
     </row>
-    <row r="181" spans="1:15">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" s="14"/>
       <c r="B181" s="15"/>
       <c r="C181" s="63"/>
@@ -28937,7 +29015,7 @@
       <c r="N181" s="15"/>
       <c r="O181" s="15"/>
     </row>
-    <row r="182" spans="1:15">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" s="14"/>
       <c r="B182" s="15"/>
       <c r="C182" s="63"/>
@@ -28954,7 +29032,7 @@
       <c r="N182" s="15"/>
       <c r="O182" s="15"/>
     </row>
-    <row r="183" spans="1:15">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" s="14"/>
       <c r="B183" s="15"/>
       <c r="C183" s="63"/>
@@ -28971,7 +29049,7 @@
       <c r="N183" s="15"/>
       <c r="O183" s="15"/>
     </row>
-    <row r="184" spans="1:15">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" s="14"/>
       <c r="B184" s="15"/>
       <c r="C184" s="63"/>
@@ -28988,7 +29066,7 @@
       <c r="N184" s="15"/>
       <c r="O184" s="15"/>
     </row>
-    <row r="185" spans="1:15">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" s="14"/>
       <c r="B185" s="15"/>
       <c r="C185" s="63"/>
@@ -29005,7 +29083,7 @@
       <c r="N185" s="15"/>
       <c r="O185" s="15"/>
     </row>
-    <row r="186" spans="1:15">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" s="14"/>
       <c r="B186" s="15"/>
       <c r="C186" s="63"/>
@@ -29022,7 +29100,7 @@
       <c r="N186" s="15"/>
       <c r="O186" s="15"/>
     </row>
-    <row r="187" spans="1:15">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" s="14"/>
       <c r="B187" s="15"/>
       <c r="C187" s="63"/>
@@ -29039,7 +29117,7 @@
       <c r="N187" s="15"/>
       <c r="O187" s="15"/>
     </row>
-    <row r="188" spans="1:15">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" s="14"/>
       <c r="B188" s="15"/>
       <c r="C188" s="63"/>
@@ -29056,7 +29134,7 @@
       <c r="N188" s="15"/>
       <c r="O188" s="15"/>
     </row>
-    <row r="189" spans="1:15">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" s="14"/>
       <c r="B189" s="15"/>
       <c r="C189" s="63"/>
@@ -29073,7 +29151,7 @@
       <c r="N189" s="15"/>
       <c r="O189" s="15"/>
     </row>
-    <row r="190" spans="1:15">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" s="14"/>
       <c r="B190" s="15"/>
       <c r="C190" s="63"/>
@@ -29090,7 +29168,7 @@
       <c r="N190" s="15"/>
       <c r="O190" s="15"/>
     </row>
-    <row r="191" spans="1:15">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" s="14"/>
       <c r="B191" s="15"/>
       <c r="C191" s="63"/>
@@ -29107,7 +29185,7 @@
       <c r="N191" s="15"/>
       <c r="O191" s="15"/>
     </row>
-    <row r="192" spans="1:15">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" s="14"/>
       <c r="B192" s="15"/>
       <c r="C192" s="63"/>
@@ -29124,7 +29202,7 @@
       <c r="N192" s="15"/>
       <c r="O192" s="15"/>
     </row>
-    <row r="193" spans="1:15">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" s="14"/>
       <c r="B193" s="15"/>
       <c r="C193" s="63"/>
@@ -29141,7 +29219,7 @@
       <c r="N193" s="15"/>
       <c r="O193" s="15"/>
     </row>
-    <row r="194" spans="1:15">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" s="14"/>
       <c r="B194" s="15"/>
       <c r="C194" s="63"/>
@@ -29158,7 +29236,7 @@
       <c r="N194" s="15"/>
       <c r="O194" s="15"/>
     </row>
-    <row r="195" spans="1:15">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" s="14"/>
       <c r="B195" s="15"/>
       <c r="C195" s="63"/>
@@ -29175,7 +29253,7 @@
       <c r="N195" s="15"/>
       <c r="O195" s="15"/>
     </row>
-    <row r="196" spans="1:15">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" s="14"/>
       <c r="B196" s="15"/>
       <c r="C196" s="63"/>
@@ -29192,7 +29270,7 @@
       <c r="N196" s="15"/>
       <c r="O196" s="15"/>
     </row>
-    <row r="197" spans="1:15">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" s="14"/>
       <c r="B197" s="15"/>
       <c r="C197" s="63"/>
@@ -29209,7 +29287,7 @@
       <c r="N197" s="15"/>
       <c r="O197" s="15"/>
     </row>
-    <row r="198" spans="1:15">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" s="14"/>
       <c r="B198" s="15"/>
       <c r="C198" s="63"/>
@@ -29226,7 +29304,7 @@
       <c r="N198" s="15"/>
       <c r="O198" s="15"/>
     </row>
-    <row r="199" spans="1:15">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" s="14"/>
       <c r="B199" s="15"/>
       <c r="C199" s="63"/>
@@ -29243,7 +29321,7 @@
       <c r="N199" s="15"/>
       <c r="O199" s="15"/>
     </row>
-    <row r="200" spans="1:15">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" s="14"/>
       <c r="B200" s="15"/>
       <c r="C200" s="63"/>
@@ -29260,7 +29338,7 @@
       <c r="N200" s="15"/>
       <c r="O200" s="15"/>
     </row>
-    <row r="201" spans="1:15">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" s="14"/>
       <c r="B201" s="15"/>
       <c r="C201" s="63"/>
@@ -29277,7 +29355,7 @@
       <c r="N201" s="15"/>
       <c r="O201" s="15"/>
     </row>
-    <row r="202" spans="1:15">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" s="14"/>
       <c r="B202" s="15"/>
       <c r="C202" s="63"/>
@@ -29294,7 +29372,7 @@
       <c r="N202" s="15"/>
       <c r="O202" s="15"/>
     </row>
-    <row r="203" spans="1:15">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" s="14"/>
       <c r="B203" s="15"/>
       <c r="C203" s="63"/>
@@ -29311,7 +29389,7 @@
       <c r="N203" s="15"/>
       <c r="O203" s="15"/>
     </row>
-    <row r="204" spans="1:15">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" s="14"/>
       <c r="B204" s="15"/>
       <c r="C204" s="63"/>
@@ -29328,7 +29406,7 @@
       <c r="N204" s="15"/>
       <c r="O204" s="15"/>
     </row>
-    <row r="205" spans="1:15">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" s="14"/>
       <c r="B205" s="15"/>
       <c r="C205" s="63"/>
@@ -29345,7 +29423,7 @@
       <c r="N205" s="15"/>
       <c r="O205" s="15"/>
     </row>
-    <row r="206" spans="1:15">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" s="14"/>
       <c r="B206" s="15"/>
       <c r="C206" s="63"/>
@@ -29362,7 +29440,7 @@
       <c r="N206" s="15"/>
       <c r="O206" s="15"/>
     </row>
-    <row r="207" spans="1:15">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" s="14"/>
       <c r="B207" s="15"/>
       <c r="C207" s="63"/>
@@ -29379,7 +29457,7 @@
       <c r="N207" s="15"/>
       <c r="O207" s="15"/>
     </row>
-    <row r="208" spans="1:15">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" s="14"/>
       <c r="B208" s="15"/>
       <c r="C208" s="63"/>
@@ -29396,7 +29474,7 @@
       <c r="N208" s="15"/>
       <c r="O208" s="15"/>
     </row>
-    <row r="209" spans="1:15">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" s="14"/>
       <c r="B209" s="15"/>
       <c r="C209" s="63"/>
@@ -29413,7 +29491,7 @@
       <c r="N209" s="15"/>
       <c r="O209" s="15"/>
     </row>
-    <row r="210" spans="1:15">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A210" s="14"/>
       <c r="B210" s="15"/>
       <c r="C210" s="63"/>
@@ -29430,7 +29508,7 @@
       <c r="N210" s="15"/>
       <c r="O210" s="15"/>
     </row>
-    <row r="211" spans="1:15">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A211" s="14"/>
       <c r="B211" s="15"/>
       <c r="C211" s="63"/>
@@ -29447,7 +29525,7 @@
       <c r="N211" s="15"/>
       <c r="O211" s="15"/>
     </row>
-    <row r="212" spans="1:15">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A212" s="14"/>
       <c r="B212" s="15"/>
       <c r="C212" s="63"/>
@@ -29464,7 +29542,7 @@
       <c r="N212" s="15"/>
       <c r="O212" s="15"/>
     </row>
-    <row r="213" spans="1:15">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A213" s="14"/>
       <c r="B213" s="15"/>
       <c r="C213" s="63"/>
@@ -29481,7 +29559,7 @@
       <c r="N213" s="15"/>
       <c r="O213" s="15"/>
     </row>
-    <row r="214" spans="1:15">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A214" s="14"/>
       <c r="B214" s="15"/>
       <c r="C214" s="63"/>
@@ -29498,7 +29576,7 @@
       <c r="N214" s="15"/>
       <c r="O214" s="15"/>
     </row>
-    <row r="215" spans="1:15">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A215" s="14"/>
       <c r="B215" s="15"/>
       <c r="C215" s="63"/>
@@ -29515,7 +29593,7 @@
       <c r="N215" s="15"/>
       <c r="O215" s="15"/>
     </row>
-    <row r="216" spans="1:15">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A216" s="14"/>
       <c r="B216" s="15"/>
       <c r="C216" s="63"/>
@@ -29532,7 +29610,7 @@
       <c r="N216" s="15"/>
       <c r="O216" s="15"/>
     </row>
-    <row r="217" spans="1:15">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A217" s="14"/>
       <c r="B217" s="15"/>
       <c r="C217" s="63"/>
@@ -29549,7 +29627,7 @@
       <c r="N217" s="15"/>
       <c r="O217" s="15"/>
     </row>
-    <row r="218" spans="1:15">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A218" s="14"/>
       <c r="B218" s="15"/>
       <c r="C218" s="63"/>
@@ -29566,7 +29644,7 @@
       <c r="N218" s="15"/>
       <c r="O218" s="15"/>
     </row>
-    <row r="219" spans="1:15">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A219" s="14"/>
       <c r="B219" s="15"/>
       <c r="C219" s="63"/>
@@ -29583,7 +29661,7 @@
       <c r="N219" s="15"/>
       <c r="O219" s="15"/>
     </row>
-    <row r="220" spans="1:15">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A220" s="14"/>
       <c r="B220" s="15"/>
       <c r="C220" s="63"/>
@@ -29600,7 +29678,7 @@
       <c r="N220" s="15"/>
       <c r="O220" s="15"/>
     </row>
-    <row r="221" spans="1:15">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A221" s="14"/>
       <c r="B221" s="15"/>
       <c r="C221" s="63"/>
@@ -29617,7 +29695,7 @@
       <c r="N221" s="15"/>
       <c r="O221" s="15"/>
     </row>
-    <row r="222" spans="1:15">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A222" s="14"/>
       <c r="B222" s="15"/>
       <c r="C222" s="63"/>
@@ -29634,7 +29712,7 @@
       <c r="N222" s="15"/>
       <c r="O222" s="15"/>
     </row>
-    <row r="223" spans="1:15">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A223" s="14"/>
       <c r="B223" s="15"/>
       <c r="C223" s="63"/>
@@ -29651,7 +29729,7 @@
       <c r="N223" s="15"/>
       <c r="O223" s="15"/>
     </row>
-    <row r="224" spans="1:15">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A224" s="14"/>
       <c r="B224" s="15"/>
       <c r="C224" s="63"/>
@@ -29668,7 +29746,7 @@
       <c r="N224" s="15"/>
       <c r="O224" s="15"/>
     </row>
-    <row r="225" spans="1:15">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A225" s="14"/>
       <c r="B225" s="15"/>
       <c r="C225" s="63"/>
@@ -29685,7 +29763,7 @@
       <c r="N225" s="15"/>
       <c r="O225" s="15"/>
     </row>
-    <row r="226" spans="1:15">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A226" s="14"/>
       <c r="B226" s="15"/>
       <c r="C226" s="63"/>
@@ -29702,7 +29780,7 @@
       <c r="N226" s="15"/>
       <c r="O226" s="15"/>
     </row>
-    <row r="227" spans="1:15">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A227" s="14"/>
       <c r="B227" s="15"/>
       <c r="C227" s="63"/>
@@ -29719,7 +29797,7 @@
       <c r="N227" s="15"/>
       <c r="O227" s="15"/>
     </row>
-    <row r="228" spans="1:15">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" s="14"/>
       <c r="B228" s="15"/>
       <c r="C228" s="63"/>
@@ -29736,7 +29814,7 @@
       <c r="N228" s="15"/>
       <c r="O228" s="15"/>
     </row>
-    <row r="229" spans="1:15">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A229" s="14"/>
       <c r="B229" s="15"/>
       <c r="C229" s="63"/>
@@ -29753,7 +29831,7 @@
       <c r="N229" s="15"/>
       <c r="O229" s="15"/>
     </row>
-    <row r="230" spans="1:15">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" s="14"/>
       <c r="B230" s="15"/>
       <c r="C230" s="63"/>
@@ -29770,7 +29848,7 @@
       <c r="N230" s="15"/>
       <c r="O230" s="15"/>
     </row>
-    <row r="231" spans="1:15">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A231" s="14"/>
       <c r="B231" s="15"/>
       <c r="C231" s="63"/>
@@ -29787,7 +29865,7 @@
       <c r="N231" s="15"/>
       <c r="O231" s="15"/>
     </row>
-    <row r="232" spans="1:15">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A232" s="14"/>
       <c r="B232" s="15"/>
       <c r="C232" s="63"/>
@@ -29804,7 +29882,7 @@
       <c r="N232" s="15"/>
       <c r="O232" s="15"/>
     </row>
-    <row r="233" spans="1:15">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A233" s="14"/>
       <c r="B233" s="15"/>
       <c r="C233" s="63"/>
@@ -29821,7 +29899,7 @@
       <c r="N233" s="15"/>
       <c r="O233" s="15"/>
     </row>
-    <row r="234" spans="1:15">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A234" s="14"/>
       <c r="B234" s="15"/>
       <c r="C234" s="63"/>
@@ -29838,7 +29916,7 @@
       <c r="N234" s="15"/>
       <c r="O234" s="15"/>
     </row>
-    <row r="235" spans="1:15">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A235" s="14"/>
       <c r="B235" s="15"/>
       <c r="C235" s="63"/>
@@ -29855,7 +29933,7 @@
       <c r="N235" s="15"/>
       <c r="O235" s="15"/>
     </row>
-    <row r="236" spans="1:15">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A236" s="14"/>
       <c r="B236" s="15"/>
       <c r="C236" s="63"/>
@@ -29872,7 +29950,7 @@
       <c r="N236" s="15"/>
       <c r="O236" s="15"/>
     </row>
-    <row r="237" spans="1:15">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A237" s="14"/>
       <c r="B237" s="15"/>
       <c r="C237" s="63"/>
@@ -29889,7 +29967,7 @@
       <c r="N237" s="15"/>
       <c r="O237" s="15"/>
     </row>
-    <row r="238" spans="1:15">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A238" s="14"/>
       <c r="B238" s="15"/>
       <c r="C238" s="63"/>
@@ -29906,7 +29984,7 @@
       <c r="N238" s="15"/>
       <c r="O238" s="15"/>
     </row>
-    <row r="239" spans="1:15">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A239" s="14"/>
       <c r="B239" s="15"/>
       <c r="C239" s="63"/>
@@ -29923,7 +30001,7 @@
       <c r="N239" s="15"/>
       <c r="O239" s="15"/>
     </row>
-    <row r="240" spans="1:15">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A240" s="14"/>
       <c r="B240" s="15"/>
       <c r="C240" s="63"/>
@@ -29940,7 +30018,7 @@
       <c r="N240" s="15"/>
       <c r="O240" s="15"/>
     </row>
-    <row r="241" spans="1:15">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A241" s="14"/>
       <c r="B241" s="15"/>
       <c r="C241" s="63"/>
@@ -29957,7 +30035,7 @@
       <c r="N241" s="15"/>
       <c r="O241" s="15"/>
     </row>
-    <row r="242" spans="1:15">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A242" s="14"/>
       <c r="B242" s="15"/>
       <c r="C242" s="63"/>
@@ -29974,7 +30052,7 @@
       <c r="N242" s="15"/>
       <c r="O242" s="15"/>
     </row>
-    <row r="243" spans="1:15">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A243" s="14"/>
       <c r="B243" s="15"/>
       <c r="C243" s="63"/>
@@ -29991,7 +30069,7 @@
       <c r="N243" s="15"/>
       <c r="O243" s="15"/>
     </row>
-    <row r="244" spans="1:15">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A244" s="14"/>
       <c r="B244" s="15"/>
       <c r="C244" s="63"/>
@@ -30008,7 +30086,7 @@
       <c r="N244" s="15"/>
       <c r="O244" s="15"/>
     </row>
-    <row r="245" spans="1:15">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A245" s="14"/>
       <c r="B245" s="15"/>
       <c r="C245" s="63"/>
@@ -30025,7 +30103,7 @@
       <c r="N245" s="15"/>
       <c r="O245" s="15"/>
     </row>
-    <row r="246" spans="1:15">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A246" s="14"/>
       <c r="B246" s="15"/>
       <c r="C246" s="63"/>
@@ -30042,7 +30120,7 @@
       <c r="N246" s="15"/>
       <c r="O246" s="15"/>
     </row>
-    <row r="247" spans="1:15">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A247" s="14"/>
       <c r="B247" s="15"/>
       <c r="C247" s="63"/>
@@ -30059,7 +30137,7 @@
       <c r="N247" s="15"/>
       <c r="O247" s="15"/>
     </row>
-    <row r="248" spans="1:15">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A248" s="14"/>
       <c r="B248" s="15"/>
       <c r="C248" s="63"/>
@@ -30076,7 +30154,7 @@
       <c r="N248" s="15"/>
       <c r="O248" s="15"/>
     </row>
-    <row r="249" spans="1:15">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A249" s="14"/>
       <c r="B249" s="15"/>
       <c r="C249" s="63"/>
@@ -30093,7 +30171,7 @@
       <c r="N249" s="15"/>
       <c r="O249" s="15"/>
     </row>
-    <row r="250" spans="1:15">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A250" s="14"/>
       <c r="B250" s="15"/>
       <c r="C250" s="63"/>
@@ -30110,7 +30188,7 @@
       <c r="N250" s="15"/>
       <c r="O250" s="15"/>
     </row>
-    <row r="251" spans="1:15">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A251" s="14"/>
       <c r="B251" s="15"/>
       <c r="C251" s="63"/>
@@ -30127,7 +30205,7 @@
       <c r="N251" s="15"/>
       <c r="O251" s="15"/>
     </row>
-    <row r="252" spans="1:15">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A252" s="14"/>
       <c r="B252" s="15"/>
       <c r="C252" s="63"/>
@@ -30144,7 +30222,7 @@
       <c r="N252" s="15"/>
       <c r="O252" s="15"/>
     </row>
-    <row r="253" spans="1:15">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A253" s="14"/>
       <c r="B253" s="15"/>
       <c r="C253" s="63"/>
@@ -30161,7 +30239,7 @@
       <c r="N253" s="15"/>
       <c r="O253" s="15"/>
     </row>
-    <row r="254" spans="1:15">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A254" s="14"/>
       <c r="B254" s="15"/>
       <c r="C254" s="63"/>
@@ -30178,7 +30256,7 @@
       <c r="N254" s="15"/>
       <c r="O254" s="15"/>
     </row>
-    <row r="255" spans="1:15">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A255" s="14"/>
       <c r="B255" s="15"/>
       <c r="C255" s="63"/>
@@ -30195,7 +30273,7 @@
       <c r="N255" s="15"/>
       <c r="O255" s="15"/>
     </row>
-    <row r="256" spans="1:15">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A256" s="14"/>
       <c r="B256" s="15"/>
       <c r="C256" s="63"/>
@@ -30212,7 +30290,7 @@
       <c r="N256" s="15"/>
       <c r="O256" s="15"/>
     </row>
-    <row r="257" spans="1:15">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A257" s="14"/>
       <c r="B257" s="15"/>
       <c r="C257" s="63"/>
@@ -30229,7 +30307,7 @@
       <c r="N257" s="15"/>
       <c r="O257" s="15"/>
     </row>
-    <row r="258" spans="1:15">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A258" s="14"/>
       <c r="B258" s="15"/>
       <c r="C258" s="63"/>
@@ -30246,7 +30324,7 @@
       <c r="N258" s="15"/>
       <c r="O258" s="15"/>
     </row>
-    <row r="259" spans="1:15">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A259" s="14"/>
       <c r="B259" s="15"/>
       <c r="C259" s="63"/>
@@ -30263,7 +30341,7 @@
       <c r="N259" s="15"/>
       <c r="O259" s="15"/>
     </row>
-    <row r="260" spans="1:15">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A260" s="14"/>
       <c r="B260" s="15"/>
       <c r="C260" s="63"/>
@@ -30280,7 +30358,7 @@
       <c r="N260" s="15"/>
       <c r="O260" s="15"/>
     </row>
-    <row r="261" spans="1:15">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A261" s="14"/>
       <c r="B261" s="15"/>
       <c r="C261" s="63"/>
@@ -30297,7 +30375,7 @@
       <c r="N261" s="15"/>
       <c r="O261" s="15"/>
     </row>
-    <row r="262" spans="1:15">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A262" s="14"/>
       <c r="B262" s="15"/>
       <c r="C262" s="63"/>
@@ -30314,7 +30392,7 @@
       <c r="N262" s="15"/>
       <c r="O262" s="15"/>
     </row>
-    <row r="263" spans="1:15">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A263" s="14"/>
       <c r="B263" s="15"/>
       <c r="C263" s="63"/>
@@ -30331,7 +30409,7 @@
       <c r="N263" s="15"/>
       <c r="O263" s="15"/>
     </row>
-    <row r="264" spans="1:15">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A264" s="14"/>
       <c r="B264" s="15"/>
       <c r="C264" s="63"/>
@@ -30348,7 +30426,7 @@
       <c r="N264" s="15"/>
       <c r="O264" s="15"/>
     </row>
-    <row r="265" spans="1:15">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A265" s="14"/>
       <c r="B265" s="15"/>
       <c r="C265" s="63"/>
@@ -30365,7 +30443,7 @@
       <c r="N265" s="15"/>
       <c r="O265" s="15"/>
     </row>
-    <row r="266" spans="1:15">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A266" s="14"/>
       <c r="B266" s="15"/>
       <c r="C266" s="63"/>
@@ -30382,7 +30460,7 @@
       <c r="N266" s="15"/>
       <c r="O266" s="15"/>
     </row>
-    <row r="267" spans="1:15">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A267" s="14"/>
       <c r="B267" s="15"/>
       <c r="C267" s="63"/>
@@ -30399,7 +30477,7 @@
       <c r="N267" s="15"/>
       <c r="O267" s="15"/>
     </row>
-    <row r="268" spans="1:15">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A268" s="14"/>
       <c r="B268" s="15"/>
       <c r="C268" s="63"/>
@@ -30416,7 +30494,7 @@
       <c r="N268" s="15"/>
       <c r="O268" s="15"/>
     </row>
-    <row r="269" spans="1:15">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A269" s="14"/>
       <c r="B269" s="15"/>
       <c r="C269" s="63"/>
@@ -30433,7 +30511,7 @@
       <c r="N269" s="15"/>
       <c r="O269" s="15"/>
     </row>
-    <row r="270" spans="1:15">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A270" s="14"/>
       <c r="B270" s="15"/>
       <c r="C270" s="63"/>
@@ -30450,7 +30528,7 @@
       <c r="N270" s="15"/>
       <c r="O270" s="15"/>
     </row>
-    <row r="271" spans="1:15">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A271" s="14"/>
       <c r="B271" s="15"/>
       <c r="C271" s="63"/>
@@ -30467,7 +30545,7 @@
       <c r="N271" s="15"/>
       <c r="O271" s="15"/>
     </row>
-    <row r="272" spans="1:15">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A272" s="14"/>
       <c r="B272" s="15"/>
       <c r="C272" s="63"/>
@@ -30484,7 +30562,7 @@
       <c r="N272" s="15"/>
       <c r="O272" s="15"/>
     </row>
-    <row r="273" spans="1:15">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A273" s="14"/>
       <c r="B273" s="15"/>
       <c r="C273" s="63"/>
@@ -30501,7 +30579,7 @@
       <c r="N273" s="15"/>
       <c r="O273" s="15"/>
     </row>
-    <row r="274" spans="1:15">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A274" s="14"/>
       <c r="B274" s="15"/>
       <c r="C274" s="63"/>
@@ -30518,7 +30596,7 @@
       <c r="N274" s="15"/>
       <c r="O274" s="15"/>
     </row>
-    <row r="275" spans="1:15">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A275" s="14"/>
       <c r="B275" s="15"/>
       <c r="C275" s="63"/>
@@ -30535,7 +30613,7 @@
       <c r="N275" s="15"/>
       <c r="O275" s="15"/>
     </row>
-    <row r="276" spans="1:15">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A276" s="14"/>
       <c r="B276" s="15"/>
       <c r="C276" s="63"/>
@@ -30552,7 +30630,7 @@
       <c r="N276" s="15"/>
       <c r="O276" s="15"/>
     </row>
-    <row r="277" spans="1:15">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A277" s="14"/>
       <c r="B277" s="15"/>
       <c r="C277" s="63"/>
@@ -30569,7 +30647,7 @@
       <c r="N277" s="15"/>
       <c r="O277" s="15"/>
     </row>
-    <row r="278" spans="1:15">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A278" s="14"/>
       <c r="B278" s="15"/>
       <c r="C278" s="63"/>
@@ -30586,7 +30664,7 @@
       <c r="N278" s="15"/>
       <c r="O278" s="15"/>
     </row>
-    <row r="279" spans="1:15">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A279" s="14"/>
       <c r="B279" s="15"/>
       <c r="C279" s="63"/>
@@ -30603,7 +30681,7 @@
       <c r="N279" s="15"/>
       <c r="O279" s="15"/>
     </row>
-    <row r="280" spans="1:15">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A280" s="14"/>
       <c r="B280" s="15"/>
       <c r="C280" s="63"/>
@@ -30620,7 +30698,7 @@
       <c r="N280" s="15"/>
       <c r="O280" s="15"/>
     </row>
-    <row r="281" spans="1:15">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A281" s="14"/>
       <c r="B281" s="15"/>
       <c r="C281" s="63"/>
@@ -30637,7 +30715,7 @@
       <c r="N281" s="15"/>
       <c r="O281" s="15"/>
     </row>
-    <row r="282" spans="1:15">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A282" s="14"/>
       <c r="B282" s="15"/>
       <c r="C282" s="63"/>
@@ -30654,7 +30732,7 @@
       <c r="N282" s="15"/>
       <c r="O282" s="15"/>
     </row>
-    <row r="283" spans="1:15">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A283" s="14"/>
       <c r="B283" s="15"/>
       <c r="C283" s="63"/>
@@ -30671,7 +30749,7 @@
       <c r="N283" s="15"/>
       <c r="O283" s="15"/>
     </row>
-    <row r="284" spans="1:15">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A284" s="14"/>
       <c r="B284" s="15"/>
       <c r="C284" s="63"/>
@@ -30688,7 +30766,7 @@
       <c r="N284" s="15"/>
       <c r="O284" s="15"/>
     </row>
-    <row r="285" spans="1:15">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A285" s="14"/>
       <c r="B285" s="15"/>
       <c r="C285" s="63"/>
@@ -30705,7 +30783,7 @@
       <c r="N285" s="15"/>
       <c r="O285" s="15"/>
     </row>
-    <row r="286" spans="1:15">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A286" s="14"/>
       <c r="B286" s="15"/>
       <c r="C286" s="63"/>
@@ -30722,7 +30800,7 @@
       <c r="N286" s="15"/>
       <c r="O286" s="15"/>
     </row>
-    <row r="287" spans="1:15">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A287" s="14"/>
       <c r="B287" s="15"/>
       <c r="C287" s="63"/>
@@ -30739,7 +30817,7 @@
       <c r="N287" s="15"/>
       <c r="O287" s="15"/>
     </row>
-    <row r="288" spans="1:15">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A288" s="14"/>
       <c r="B288" s="15"/>
       <c r="C288" s="63"/>
@@ -30756,7 +30834,7 @@
       <c r="N288" s="15"/>
       <c r="O288" s="15"/>
     </row>
-    <row r="289" spans="1:15">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A289" s="14"/>
       <c r="B289" s="15"/>
       <c r="C289" s="63"/>
@@ -30773,7 +30851,7 @@
       <c r="N289" s="15"/>
       <c r="O289" s="15"/>
     </row>
-    <row r="290" spans="1:15">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A290" s="14"/>
       <c r="B290" s="15"/>
       <c r="C290" s="63"/>
@@ -30790,7 +30868,7 @@
       <c r="N290" s="15"/>
       <c r="O290" s="15"/>
     </row>
-    <row r="291" spans="1:15">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A291" s="14"/>
       <c r="B291" s="15"/>
       <c r="C291" s="63"/>
@@ -30807,7 +30885,7 @@
       <c r="N291" s="15"/>
       <c r="O291" s="15"/>
     </row>
-    <row r="292" spans="1:15">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A292" s="14"/>
       <c r="B292" s="15"/>
       <c r="C292" s="63"/>
@@ -30824,7 +30902,7 @@
       <c r="N292" s="15"/>
       <c r="O292" s="15"/>
     </row>
-    <row r="293" spans="1:15">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A293" s="14"/>
       <c r="B293" s="15"/>
       <c r="C293" s="63"/>
@@ -30841,7 +30919,7 @@
       <c r="N293" s="15"/>
       <c r="O293" s="15"/>
     </row>
-    <row r="294" spans="1:15">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A294" s="14"/>
       <c r="B294" s="15"/>
       <c r="C294" s="63"/>
@@ -30858,7 +30936,7 @@
       <c r="N294" s="15"/>
       <c r="O294" s="15"/>
     </row>
-    <row r="295" spans="1:15">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A295" s="14"/>
       <c r="B295" s="15"/>
       <c r="C295" s="63"/>
@@ -30875,7 +30953,7 @@
       <c r="N295" s="15"/>
       <c r="O295" s="15"/>
     </row>
-    <row r="296" spans="1:15">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A296" s="14"/>
       <c r="B296" s="15"/>
       <c r="C296" s="63"/>
@@ -30892,7 +30970,7 @@
       <c r="N296" s="15"/>
       <c r="O296" s="15"/>
     </row>
-    <row r="297" spans="1:15">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A297" s="14"/>
       <c r="B297" s="15"/>
       <c r="C297" s="63"/>
@@ -30909,7 +30987,7 @@
       <c r="N297" s="15"/>
       <c r="O297" s="15"/>
     </row>
-    <row r="298" spans="1:15">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A298" s="14"/>
       <c r="B298" s="15"/>
       <c r="C298" s="63"/>
@@ -30926,7 +31004,7 @@
       <c r="N298" s="15"/>
       <c r="O298" s="15"/>
     </row>
-    <row r="299" spans="1:15">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A299" s="14"/>
       <c r="B299" s="15"/>
       <c r="C299" s="63"/>
@@ -30943,7 +31021,7 @@
       <c r="N299" s="15"/>
       <c r="O299" s="15"/>
     </row>
-    <row r="300" spans="1:15">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A300" s="14"/>
       <c r="B300" s="15"/>
       <c r="C300" s="63"/>
@@ -30960,7 +31038,7 @@
       <c r="N300" s="15"/>
       <c r="O300" s="15"/>
     </row>
-    <row r="301" spans="1:15">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A301" s="14"/>
       <c r="B301" s="15"/>
       <c r="C301" s="63"/>
@@ -30977,7 +31055,7 @@
       <c r="N301" s="15"/>
       <c r="O301" s="15"/>
     </row>
-    <row r="302" spans="1:15">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A302" s="14"/>
       <c r="B302" s="15"/>
       <c r="C302" s="63"/>
@@ -30994,7 +31072,7 @@
       <c r="N302" s="15"/>
       <c r="O302" s="15"/>
     </row>
-    <row r="303" spans="1:15">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A303" s="14"/>
       <c r="B303" s="15"/>
       <c r="C303" s="63"/>
@@ -31011,7 +31089,7 @@
       <c r="N303" s="15"/>
       <c r="O303" s="15"/>
     </row>
-    <row r="304" spans="1:15">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A304" s="14"/>
       <c r="B304" s="15"/>
       <c r="C304" s="63"/>
@@ -31028,7 +31106,7 @@
       <c r="N304" s="15"/>
       <c r="O304" s="15"/>
     </row>
-    <row r="305" spans="1:15">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A305" s="14"/>
       <c r="B305" s="15"/>
       <c r="C305" s="63"/>
@@ -31045,7 +31123,7 @@
       <c r="N305" s="15"/>
       <c r="O305" s="15"/>
     </row>
-    <row r="306" spans="1:15">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A306" s="14"/>
       <c r="B306" s="15"/>
       <c r="C306" s="63"/>
@@ -31062,7 +31140,7 @@
       <c r="N306" s="15"/>
       <c r="O306" s="15"/>
     </row>
-    <row r="307" spans="1:15">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A307" s="14"/>
       <c r="B307" s="15"/>
       <c r="C307" s="63"/>
@@ -31079,7 +31157,7 @@
       <c r="N307" s="15"/>
       <c r="O307" s="15"/>
     </row>
-    <row r="308" spans="1:15">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A308" s="14"/>
       <c r="B308" s="15"/>
       <c r="C308" s="63"/>
@@ -31096,7 +31174,7 @@
       <c r="N308" s="15"/>
       <c r="O308" s="15"/>
     </row>
-    <row r="309" spans="1:15">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A309" s="14"/>
       <c r="B309" s="15"/>
       <c r="C309" s="63"/>
@@ -31113,7 +31191,7 @@
       <c r="N309" s="15"/>
       <c r="O309" s="15"/>
     </row>
-    <row r="310" spans="1:15">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A310" s="14"/>
       <c r="B310" s="15"/>
       <c r="C310" s="63"/>
@@ -31130,7 +31208,7 @@
       <c r="N310" s="15"/>
       <c r="O310" s="15"/>
     </row>
-    <row r="311" spans="1:15">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A311" s="14"/>
       <c r="B311" s="15"/>
       <c r="C311" s="63"/>
@@ -31147,7 +31225,7 @@
       <c r="N311" s="15"/>
       <c r="O311" s="15"/>
     </row>
-    <row r="312" spans="1:15">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A312" s="14"/>
       <c r="B312" s="15"/>
       <c r="C312" s="63"/>
@@ -31164,7 +31242,7 @@
       <c r="N312" s="15"/>
       <c r="O312" s="15"/>
     </row>
-    <row r="313" spans="1:15">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A313" s="14"/>
       <c r="B313" s="15"/>
       <c r="C313" s="63"/>
@@ -31181,7 +31259,7 @@
       <c r="N313" s="15"/>
       <c r="O313" s="15"/>
     </row>
-    <row r="314" spans="1:15">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A314" s="14"/>
       <c r="B314" s="15"/>
       <c r="C314" s="63"/>
@@ -31198,7 +31276,7 @@
       <c r="N314" s="15"/>
       <c r="O314" s="15"/>
     </row>
-    <row r="315" spans="1:15">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A315" s="14"/>
       <c r="B315" s="15"/>
       <c r="C315" s="63"/>
@@ -31215,7 +31293,7 @@
       <c r="N315" s="15"/>
       <c r="O315" s="15"/>
     </row>
-    <row r="316" spans="1:15">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A316" s="14"/>
       <c r="B316" s="15"/>
       <c r="C316" s="63"/>
@@ -31232,7 +31310,7 @@
       <c r="N316" s="15"/>
       <c r="O316" s="15"/>
     </row>
-    <row r="317" spans="1:15">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A317" s="14"/>
       <c r="B317" s="15"/>
       <c r="C317" s="63"/>
@@ -31249,7 +31327,7 @@
       <c r="N317" s="15"/>
       <c r="O317" s="15"/>
     </row>
-    <row r="318" spans="1:15">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A318" s="14"/>
       <c r="B318" s="15"/>
       <c r="C318" s="63"/>
@@ -31266,7 +31344,7 @@
       <c r="N318" s="15"/>
       <c r="O318" s="15"/>
     </row>
-    <row r="319" spans="1:15">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A319" s="14"/>
       <c r="B319" s="15"/>
       <c r="C319" s="63"/>
@@ -31283,7 +31361,7 @@
       <c r="N319" s="15"/>
       <c r="O319" s="15"/>
     </row>
-    <row r="320" spans="1:15">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A320" s="14"/>
       <c r="B320" s="15"/>
       <c r="C320" s="63"/>
@@ -31300,7 +31378,7 @@
       <c r="N320" s="15"/>
       <c r="O320" s="15"/>
     </row>
-    <row r="321" spans="1:15">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A321" s="14"/>
       <c r="B321" s="15"/>
       <c r="C321" s="63"/>
@@ -31317,7 +31395,7 @@
       <c r="N321" s="15"/>
       <c r="O321" s="15"/>
     </row>
-    <row r="322" spans="1:15">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A322" s="14"/>
       <c r="B322" s="15"/>
       <c r="C322" s="63"/>
@@ -31334,7 +31412,7 @@
       <c r="N322" s="15"/>
       <c r="O322" s="15"/>
     </row>
-    <row r="323" spans="1:15">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A323" s="14"/>
       <c r="B323" s="15"/>
       <c r="C323" s="63"/>
@@ -31351,7 +31429,7 @@
       <c r="N323" s="15"/>
       <c r="O323" s="15"/>
     </row>
-    <row r="324" spans="1:15">
+    <row r="324" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A324" s="14"/>
       <c r="B324" s="15"/>
       <c r="C324" s="63"/>
@@ -31368,7 +31446,7 @@
       <c r="N324" s="15"/>
       <c r="O324" s="15"/>
     </row>
-    <row r="325" spans="1:15">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A325" s="14"/>
       <c r="B325" s="15"/>
       <c r="C325" s="63"/>
@@ -31385,7 +31463,7 @@
       <c r="N325" s="15"/>
       <c r="O325" s="15"/>
     </row>
-    <row r="326" spans="1:15">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A326" s="14"/>
       <c r="B326" s="15"/>
       <c r="C326" s="63"/>
@@ -31402,7 +31480,7 @@
       <c r="N326" s="15"/>
       <c r="O326" s="15"/>
     </row>
-    <row r="327" spans="1:15">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A327" s="14"/>
       <c r="B327" s="15"/>
       <c r="C327" s="63"/>
@@ -31419,7 +31497,7 @@
       <c r="N327" s="15"/>
       <c r="O327" s="15"/>
     </row>
-    <row r="328" spans="1:15">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A328" s="14"/>
       <c r="B328" s="15"/>
       <c r="C328" s="63"/>
@@ -31436,7 +31514,7 @@
       <c r="N328" s="15"/>
       <c r="O328" s="15"/>
     </row>
-    <row r="329" spans="1:15">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A329" s="14"/>
       <c r="B329" s="15"/>
       <c r="C329" s="63"/>
@@ -31453,7 +31531,7 @@
       <c r="N329" s="15"/>
       <c r="O329" s="15"/>
     </row>
-    <row r="330" spans="1:15">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A330" s="14"/>
       <c r="B330" s="15"/>
       <c r="C330" s="63"/>
@@ -31470,7 +31548,7 @@
       <c r="N330" s="15"/>
       <c r="O330" s="15"/>
     </row>
-    <row r="331" spans="1:15">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A331" s="14"/>
       <c r="B331" s="15"/>
       <c r="C331" s="63"/>
@@ -31487,7 +31565,7 @@
       <c r="N331" s="15"/>
       <c r="O331" s="15"/>
     </row>
-    <row r="332" spans="1:15">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A332" s="14"/>
       <c r="B332" s="15"/>
       <c r="C332" s="63"/>
@@ -31504,7 +31582,7 @@
       <c r="N332" s="15"/>
       <c r="O332" s="15"/>
     </row>
-    <row r="333" spans="1:15">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A333" s="14"/>
       <c r="B333" s="15"/>
       <c r="C333" s="63"/>
@@ -31521,7 +31599,7 @@
       <c r="N333" s="15"/>
       <c r="O333" s="15"/>
     </row>
-    <row r="334" spans="1:15">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A334" s="14"/>
       <c r="B334" s="15"/>
       <c r="C334" s="63"/>
@@ -31538,7 +31616,7 @@
       <c r="N334" s="15"/>
       <c r="O334" s="15"/>
     </row>
-    <row r="335" spans="1:15">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A335" s="14"/>
       <c r="B335" s="15"/>
       <c r="C335" s="63"/>
@@ -31555,7 +31633,7 @@
       <c r="N335" s="15"/>
       <c r="O335" s="15"/>
     </row>
-    <row r="336" spans="1:15">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A336" s="14"/>
       <c r="B336" s="15"/>
       <c r="C336" s="63"/>
@@ -31572,7 +31650,7 @@
       <c r="N336" s="15"/>
       <c r="O336" s="15"/>
     </row>
-    <row r="337" spans="1:15">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A337" s="14"/>
       <c r="B337" s="15"/>
       <c r="C337" s="63"/>
@@ -31589,9 +31667,10 @@
       <c r="N337" s="15"/>
       <c r="O337" s="15"/>
     </row>
-    <row r="338" spans="1:15">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A338" s="14"/>
       <c r="B338" s="15"/>
+      <c r="C338" s="63"/>
       <c r="D338" s="14"/>
       <c r="E338" s="14"/>
       <c r="F338" s="14"/>
@@ -31605,30 +31684,49 @@
       <c r="N338" s="15"/>
       <c r="O338" s="15"/>
     </row>
+    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A339" s="14"/>
+      <c r="B339" s="15"/>
+      <c r="D339" s="14"/>
+      <c r="E339" s="14"/>
+      <c r="F339" s="14"/>
+      <c r="G339" s="30"/>
+      <c r="H339" s="30"/>
+      <c r="I339" s="30"/>
+      <c r="J339" s="14"/>
+      <c r="K339" s="14"/>
+      <c r="L339" s="14"/>
+      <c r="M339" s="15"/>
+      <c r="N339" s="15"/>
+      <c r="O339" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A91:O91"/>
+    <mergeCell ref="A92:O92"/>
+    <mergeCell ref="A74:O74"/>
+    <mergeCell ref="A60:O60"/>
+    <mergeCell ref="A75:O75"/>
     <mergeCell ref="A59:O59"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A19:O19"/>
     <mergeCell ref="A44:O44"/>
     <mergeCell ref="A45:O45"/>
-    <mergeCell ref="A91:O91"/>
-    <mergeCell ref="A92:O92"/>
-    <mergeCell ref="A74:O74"/>
-    <mergeCell ref="A60:O60"/>
-    <mergeCell ref="A75:O75"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L54:L58 L11:L15 L69:L73 L23:L24 L31:L32 L17:L18 L7:L9 L65:L67 L50:L52 L26:L29 L83:L86 L89 L79:L81 L96:L98 L100:L104" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K54:K58 K69:K73 K65:K67 K7:K9 K50:K52 K11:K18 K83:K89 K79:K81 K23:K43 K96:K98 K100:K104" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K54:K58 K69:K73 K65:K67 K7:K9 K50:K52 K11:K18 K83:K89 K79:K81 K23:K43 K96:K98 K100:K106" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
       <formula1>"Field,Cross Field,Cross Form"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J54:J58 J69:J73 J65:J67 J7:J9 J50:J52 J11:J18 J83:J89 J79:J81 J23:J43 J96:J98 J100:J104" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J54:J58 J69:J73 J65:J67 J7:J9 J50:J52 J11:J18 J83:J89 J79:J81 J23:J43 J96:J98 J100:J106" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
       <formula1>"Error,Warning"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L105" xr:uid="{09356DAA-76AD-4A0A-A6BF-2F20998BA0A3}">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31689,6 +31787,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Word document" ma:contentTypeID="0x010100852E11B2A94E4937B655CB4FCD918453006DFD5C59A7CB45AAB5046F3899BB7DEC00F397826DF95DEB4B8DB89BEACF2240F1" ma:contentTypeVersion="79" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2efa76ee5d5cd602cc18ca32df57176e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9394a98c30c487d0596bd1768260a67a" ns2:_="">
     <xsd:import namespace="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
@@ -31908,23 +32015,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8031746-25E9-4E51-ABEB-14F1D0CC1382}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8031746-25E9-4E51-ABEB-14F1D0CC1382}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates to validation sheet
</commit_message>
<xml_diff>
--- a/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
+++ b/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24A43AF-24B4-4491-A274-673E10646814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF1FBC3D-50AB-466F-8EDB-FD1064147B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="7530" windowWidth="19365" windowHeight="2820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27960" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -1099,6 +1099,18 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1126,9 +1138,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1138,17 +1147,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -21850,14 +21850,14 @@
   <dimension ref="B8:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="13.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="87" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="74" customWidth="1"/>
     <col min="4" max="4" width="51.140625" style="7" customWidth="1"/>
     <col min="5" max="5" width="55.42578125" style="68" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" style="7" customWidth="1"/>
@@ -21865,18 +21865,18 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
@@ -21917,71 +21917,71 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="72">
+      <c r="B14" s="76">
         <v>0.12</v>
       </c>
-      <c r="C14" s="84">
+      <c r="C14" s="71">
         <v>169</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="75">
+      <c r="E14" s="79">
         <v>45218</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="73"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="34" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="76"/>
+      <c r="E15" s="80"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="73"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="76"/>
+      <c r="E16" s="80"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="73"/>
-      <c r="C17" s="84" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="71" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="76"/>
+      <c r="E17" s="80"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="74"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="77"/>
+      <c r="E18" s="81"/>
     </row>
     <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="59">
         <v>0.13</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="71" t="s">
         <v>183</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>182</v>
       </c>
       <c r="E19" s="70">
-        <v>45638</v>
+        <v>45272</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -22124,7 +22124,7 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="61"/>
-      <c r="C43" s="85"/>
+      <c r="C43" s="72"/>
       <c r="D43" s="39"/>
       <c r="E43" s="66"/>
     </row>
@@ -22160,7 +22160,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="62"/>
-      <c r="C49" s="86"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="36"/>
       <c r="E49" s="65"/>
     </row>
@@ -22367,43 +22367,43 @@
       <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="80"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="87"/>
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="83"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="86"/>
       <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -23165,23 +23165,23 @@
       <c r="P18" s="24"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="83"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="86"/>
       <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24410,43 +24410,43 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="78" t="s">
+      <c r="A46" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="79"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="79"/>
-      <c r="G46" s="79"/>
-      <c r="H46" s="79"/>
-      <c r="I46" s="79"/>
-      <c r="J46" s="79"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
-      <c r="M46" s="79"/>
-      <c r="N46" s="79"/>
-      <c r="O46" s="80"/>
+      <c r="B46" s="83"/>
+      <c r="C46" s="83"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="83"/>
+      <c r="M46" s="83"/>
+      <c r="N46" s="83"/>
+      <c r="O46" s="87"/>
       <c r="P46" s="13"/>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="82"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="82"/>
-      <c r="M47" s="82"/>
-      <c r="N47" s="82"/>
-      <c r="O47" s="83"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="85"/>
+      <c r="D47" s="85"/>
+      <c r="E47" s="85"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="85"/>
+      <c r="H47" s="85"/>
+      <c r="I47" s="85"/>
+      <c r="J47" s="85"/>
+      <c r="K47" s="85"/>
+      <c r="L47" s="85"/>
+      <c r="M47" s="85"/>
+      <c r="N47" s="85"/>
+      <c r="O47" s="86"/>
       <c r="P47" s="13"/>
     </row>
     <row r="48" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -25114,43 +25114,43 @@
       </c>
     </row>
     <row r="61" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="78" t="s">
+      <c r="A61" s="82" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="79"/>
-      <c r="C61" s="79"/>
-      <c r="D61" s="79"/>
-      <c r="E61" s="79"/>
-      <c r="F61" s="79"/>
-      <c r="G61" s="79"/>
-      <c r="H61" s="79"/>
-      <c r="I61" s="79"/>
-      <c r="J61" s="79"/>
-      <c r="K61" s="79"/>
-      <c r="L61" s="79"/>
-      <c r="M61" s="79"/>
-      <c r="N61" s="79"/>
-      <c r="O61" s="80"/>
+      <c r="B61" s="83"/>
+      <c r="C61" s="83"/>
+      <c r="D61" s="83"/>
+      <c r="E61" s="83"/>
+      <c r="F61" s="83"/>
+      <c r="G61" s="83"/>
+      <c r="H61" s="83"/>
+      <c r="I61" s="83"/>
+      <c r="J61" s="83"/>
+      <c r="K61" s="83"/>
+      <c r="L61" s="83"/>
+      <c r="M61" s="83"/>
+      <c r="N61" s="83"/>
+      <c r="O61" s="87"/>
       <c r="P61" s="13"/>
     </row>
     <row r="62" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="81" t="s">
+      <c r="A62" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="82"/>
-      <c r="C62" s="82"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="82"/>
-      <c r="F62" s="82"/>
-      <c r="G62" s="82"/>
-      <c r="H62" s="82"/>
-      <c r="I62" s="82"/>
-      <c r="J62" s="82"/>
-      <c r="K62" s="82"/>
-      <c r="L62" s="82"/>
-      <c r="M62" s="82"/>
-      <c r="N62" s="82"/>
-      <c r="O62" s="83"/>
+      <c r="B62" s="85"/>
+      <c r="C62" s="85"/>
+      <c r="D62" s="85"/>
+      <c r="E62" s="85"/>
+      <c r="F62" s="85"/>
+      <c r="G62" s="85"/>
+      <c r="H62" s="85"/>
+      <c r="I62" s="85"/>
+      <c r="J62" s="85"/>
+      <c r="K62" s="85"/>
+      <c r="L62" s="85"/>
+      <c r="M62" s="85"/>
+      <c r="N62" s="85"/>
+      <c r="O62" s="86"/>
       <c r="P62" s="13"/>
     </row>
     <row r="63" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -25818,23 +25818,23 @@
       </c>
     </row>
     <row r="76" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="78" t="s">
+      <c r="A76" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="B76" s="79"/>
-      <c r="C76" s="79"/>
-      <c r="D76" s="79"/>
-      <c r="E76" s="79"/>
-      <c r="F76" s="79"/>
-      <c r="G76" s="79"/>
-      <c r="H76" s="79"/>
-      <c r="I76" s="79"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="79"/>
-      <c r="L76" s="79"/>
-      <c r="M76" s="79"/>
-      <c r="N76" s="79"/>
-      <c r="O76" s="79"/>
+      <c r="B76" s="83"/>
+      <c r="C76" s="83"/>
+      <c r="D76" s="83"/>
+      <c r="E76" s="83"/>
+      <c r="F76" s="83"/>
+      <c r="G76" s="83"/>
+      <c r="H76" s="83"/>
+      <c r="I76" s="83"/>
+      <c r="J76" s="83"/>
+      <c r="K76" s="83"/>
+      <c r="L76" s="83"/>
+      <c r="M76" s="83"/>
+      <c r="N76" s="83"/>
+      <c r="O76" s="83"/>
       <c r="P76" s="13"/>
       <c r="Q76" s="13"/>
       <c r="R76" s="13"/>
@@ -25887,23 +25887,23 @@
       <c r="BM76" s="13"/>
     </row>
     <row r="77" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="81" t="s">
+      <c r="A77" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B77" s="82"/>
-      <c r="C77" s="82"/>
-      <c r="D77" s="82"/>
-      <c r="E77" s="82"/>
-      <c r="F77" s="82"/>
-      <c r="G77" s="82"/>
-      <c r="H77" s="82"/>
-      <c r="I77" s="82"/>
-      <c r="J77" s="82"/>
-      <c r="K77" s="82"/>
-      <c r="L77" s="82"/>
-      <c r="M77" s="82"/>
-      <c r="N77" s="82"/>
-      <c r="O77" s="82"/>
+      <c r="B77" s="85"/>
+      <c r="C77" s="85"/>
+      <c r="D77" s="85"/>
+      <c r="E77" s="85"/>
+      <c r="F77" s="85"/>
+      <c r="G77" s="85"/>
+      <c r="H77" s="85"/>
+      <c r="I77" s="85"/>
+      <c r="J77" s="85"/>
+      <c r="K77" s="85"/>
+      <c r="L77" s="85"/>
+      <c r="M77" s="85"/>
+      <c r="N77" s="85"/>
+      <c r="O77" s="85"/>
       <c r="P77" s="13"/>
       <c r="Q77" s="13"/>
       <c r="R77" s="13"/>
@@ -27256,23 +27256,23 @@
       </c>
     </row>
     <row r="92" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="78" t="s">
+      <c r="A92" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="B92" s="79"/>
-      <c r="C92" s="79"/>
-      <c r="D92" s="79"/>
-      <c r="E92" s="79"/>
-      <c r="F92" s="79"/>
-      <c r="G92" s="79"/>
-      <c r="H92" s="79"/>
-      <c r="I92" s="79"/>
-      <c r="J92" s="79"/>
-      <c r="K92" s="79"/>
-      <c r="L92" s="79"/>
-      <c r="M92" s="79"/>
-      <c r="N92" s="79"/>
-      <c r="O92" s="79"/>
+      <c r="B92" s="83"/>
+      <c r="C92" s="83"/>
+      <c r="D92" s="83"/>
+      <c r="E92" s="83"/>
+      <c r="F92" s="83"/>
+      <c r="G92" s="83"/>
+      <c r="H92" s="83"/>
+      <c r="I92" s="83"/>
+      <c r="J92" s="83"/>
+      <c r="K92" s="83"/>
+      <c r="L92" s="83"/>
+      <c r="M92" s="83"/>
+      <c r="N92" s="83"/>
+      <c r="O92" s="83"/>
       <c r="P92" s="13"/>
       <c r="Q92" s="13"/>
       <c r="R92" s="13"/>
@@ -27325,23 +27325,23 @@
       <c r="BM92" s="13"/>
     </row>
     <row r="93" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="81" t="s">
+      <c r="A93" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B93" s="82"/>
-      <c r="C93" s="82"/>
-      <c r="D93" s="82"/>
-      <c r="E93" s="82"/>
-      <c r="F93" s="82"/>
-      <c r="G93" s="82"/>
-      <c r="H93" s="82"/>
-      <c r="I93" s="82"/>
-      <c r="J93" s="82"/>
-      <c r="K93" s="82"/>
-      <c r="L93" s="82"/>
-      <c r="M93" s="82"/>
-      <c r="N93" s="82"/>
-      <c r="O93" s="82"/>
+      <c r="B93" s="85"/>
+      <c r="C93" s="85"/>
+      <c r="D93" s="85"/>
+      <c r="E93" s="85"/>
+      <c r="F93" s="85"/>
+      <c r="G93" s="85"/>
+      <c r="H93" s="85"/>
+      <c r="I93" s="85"/>
+      <c r="J93" s="85"/>
+      <c r="K93" s="85"/>
+      <c r="L93" s="85"/>
+      <c r="M93" s="85"/>
+      <c r="N93" s="85"/>
+      <c r="O93" s="85"/>
     </row>
     <row r="94" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A94" s="44">
@@ -31963,17 +31963,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:O92"/>
-    <mergeCell ref="A93:O93"/>
-    <mergeCell ref="A76:O76"/>
-    <mergeCell ref="A62:O62"/>
-    <mergeCell ref="A77:O77"/>
     <mergeCell ref="A61:O61"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A19:O19"/>
     <mergeCell ref="A46:O46"/>
     <mergeCell ref="A47:O47"/>
+    <mergeCell ref="A92:O92"/>
+    <mergeCell ref="A93:O93"/>
+    <mergeCell ref="A76:O76"/>
+    <mergeCell ref="A62:O62"/>
+    <mergeCell ref="A77:O77"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
@@ -32002,6 +32002,58 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l29cd52af9b640b690e3347aa75f97a9>
+    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ade64af1c6a24cfdbe8da7f962b31d74>
+    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
+        </TermInfo>
+      </Terms>
+    </e62af2f156934d1aab35222180c5fbb1>
+    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
+        </TermInfo>
+      </Terms>
+    </nb82aa7489a64919aab5fd247ffa0d1e>
+    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
+        </TermInfo>
+      </Terms>
+    </f62107d924a7469492625f91956e46a6>
+    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e9be08524f454d8b979862330e952271>
+    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Value>97</Value>
+      <Value>45</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <UserInfo>
+        <DisplayName>Hunt, Martin</DisplayName>
+        <AccountId>118</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Word document" ma:contentTypeID="0x010100852E11B2A94E4937B655CB4FCD918453006DFD5C59A7CB45AAB5046F3899BB7DEC00F397826DF95DEB4B8DB89BEACF2240F1" ma:contentTypeVersion="79" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2efa76ee5d5cd602cc18ca32df57176e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9394a98c30c487d0596bd1768260a67a" ns2:_="">
     <xsd:import namespace="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
@@ -32221,58 +32273,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l29cd52af9b640b690e3347aa75f97a9>
-    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ade64af1c6a24cfdbe8da7f962b31d74>
-    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
-        </TermInfo>
-      </Terms>
-    </e62af2f156934d1aab35222180c5fbb1>
-    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
-        </TermInfo>
-      </Terms>
-    </nb82aa7489a64919aab5fd247ffa0d1e>
-    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
-        </TermInfo>
-      </Terms>
-    </f62107d924a7469492625f91956e46a6>
-    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e9be08524f454d8b979862330e952271>
-    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Value>97</Value>
-      <Value>45</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <UserInfo>
-        <DisplayName>Hunt, Martin</DisplayName>
-        <AccountId>118</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
   <ds:schemaRefs>
@@ -32282,6 +32282,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8031746-25E9-4E51-ABEB-14F1D0CC1382}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32297,14 +32307,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ERR add validation rule for RPN service error
</commit_message>
<xml_diff>
--- a/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
+++ b/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91288C5E-7BC8-4763-8F8E-10F76E516E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291695A2-33FA-4A51-A96A-BD9093EF72A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="192">
   <si>
     <t xml:space="preserve">Latest Version History </t>
   </si>
@@ -617,6 +617,15 @@
   </si>
   <si>
     <t xml:space="preserve">Advance Payment reconciliation </t>
+  </si>
+  <si>
+    <t>No record found for Employer Registration Id provided.</t>
+  </si>
+  <si>
+    <t>No record found for Employer Registration Id provided due to RPN service error.</t>
+  </si>
+  <si>
+    <t>EmployerRegistrationId</t>
   </si>
 </sst>
 </file>
@@ -1247,6 +1256,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1254,9 +1266,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -22413,10 +22422,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM342"/>
+  <dimension ref="A1:BM343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -22501,27 +22510,27 @@
       <c r="L2" s="96"/>
       <c r="M2" s="96"/>
       <c r="N2" s="96"/>
-      <c r="O2" s="100"/>
+      <c r="O2" s="97"/>
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="99"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="100"/>
       <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -23283,23 +23292,23 @@
       <c r="P18" s="24"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="98"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="98"/>
-      <c r="O19" s="99"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="99"/>
+      <c r="N19" s="99"/>
+      <c r="O19" s="100"/>
       <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24642,23 +24651,23 @@
       <c r="P48" s="13"/>
     </row>
     <row r="49" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="97" t="s">
+      <c r="A49" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="98"/>
-      <c r="C49" s="98"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="98"/>
-      <c r="I49" s="98"/>
-      <c r="J49" s="98"/>
-      <c r="K49" s="98"/>
-      <c r="L49" s="98"/>
-      <c r="M49" s="98"/>
-      <c r="N49" s="98"/>
-      <c r="O49" s="99"/>
+      <c r="B49" s="99"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="99"/>
+      <c r="F49" s="99"/>
+      <c r="G49" s="99"/>
+      <c r="H49" s="99"/>
+      <c r="I49" s="99"/>
+      <c r="J49" s="99"/>
+      <c r="K49" s="99"/>
+      <c r="L49" s="99"/>
+      <c r="M49" s="99"/>
+      <c r="N49" s="99"/>
+      <c r="O49" s="100"/>
       <c r="P49" s="13"/>
     </row>
     <row r="50" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -25342,27 +25351,27 @@
       <c r="L63" s="96"/>
       <c r="M63" s="96"/>
       <c r="N63" s="96"/>
-      <c r="O63" s="100"/>
+      <c r="O63" s="97"/>
       <c r="P63" s="13"/>
     </row>
     <row r="64" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="97" t="s">
+      <c r="A64" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B64" s="98"/>
-      <c r="C64" s="98"/>
-      <c r="D64" s="98"/>
-      <c r="E64" s="98"/>
-      <c r="F64" s="98"/>
-      <c r="G64" s="98"/>
-      <c r="H64" s="98"/>
-      <c r="I64" s="98"/>
-      <c r="J64" s="98"/>
-      <c r="K64" s="98"/>
-      <c r="L64" s="98"/>
-      <c r="M64" s="98"/>
-      <c r="N64" s="98"/>
-      <c r="O64" s="99"/>
+      <c r="B64" s="99"/>
+      <c r="C64" s="99"/>
+      <c r="D64" s="99"/>
+      <c r="E64" s="99"/>
+      <c r="F64" s="99"/>
+      <c r="G64" s="99"/>
+      <c r="H64" s="99"/>
+      <c r="I64" s="99"/>
+      <c r="J64" s="99"/>
+      <c r="K64" s="99"/>
+      <c r="L64" s="99"/>
+      <c r="M64" s="99"/>
+      <c r="N64" s="99"/>
+      <c r="O64" s="100"/>
       <c r="P64" s="13"/>
     </row>
     <row r="65" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -26099,23 +26108,23 @@
       <c r="BM78" s="13"/>
     </row>
     <row r="79" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="97" t="s">
+      <c r="A79" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B79" s="98"/>
-      <c r="C79" s="98"/>
-      <c r="D79" s="98"/>
-      <c r="E79" s="98"/>
-      <c r="F79" s="98"/>
-      <c r="G79" s="98"/>
-      <c r="H79" s="98"/>
-      <c r="I79" s="98"/>
-      <c r="J79" s="98"/>
-      <c r="K79" s="98"/>
-      <c r="L79" s="98"/>
-      <c r="M79" s="98"/>
-      <c r="N79" s="98"/>
-      <c r="O79" s="98"/>
+      <c r="B79" s="99"/>
+      <c r="C79" s="99"/>
+      <c r="D79" s="99"/>
+      <c r="E79" s="99"/>
+      <c r="F79" s="99"/>
+      <c r="G79" s="99"/>
+      <c r="H79" s="99"/>
+      <c r="I79" s="99"/>
+      <c r="J79" s="99"/>
+      <c r="K79" s="99"/>
+      <c r="L79" s="99"/>
+      <c r="M79" s="99"/>
+      <c r="N79" s="99"/>
+      <c r="O79" s="99"/>
       <c r="P79" s="13"/>
       <c r="Q79" s="13"/>
       <c r="R79" s="13"/>
@@ -27467,197 +27476,197 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="95" t="s">
+    <row r="94" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>175</v>
+      </c>
+      <c r="B94" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D94" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F94" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G94" s="16">
+        <v>200</v>
+      </c>
+      <c r="H94" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I94" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L94" s="4">
+        <v>3015</v>
+      </c>
+      <c r="M94" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="N94" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="O94" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="95" t="s">
         <v>171</v>
       </c>
-      <c r="B94" s="96"/>
-      <c r="C94" s="96"/>
-      <c r="D94" s="96"/>
-      <c r="E94" s="96"/>
-      <c r="F94" s="96"/>
-      <c r="G94" s="96"/>
-      <c r="H94" s="96"/>
-      <c r="I94" s="96"/>
-      <c r="J94" s="96"/>
-      <c r="K94" s="96"/>
-      <c r="L94" s="96"/>
-      <c r="M94" s="96"/>
-      <c r="N94" s="96"/>
-      <c r="O94" s="96"/>
-      <c r="P94" s="13"/>
-      <c r="Q94" s="13"/>
-      <c r="R94" s="13"/>
-      <c r="S94" s="13"/>
-      <c r="T94" s="13"/>
-      <c r="U94" s="13"/>
-      <c r="V94" s="13"/>
-      <c r="W94" s="13"/>
-      <c r="X94" s="13"/>
-      <c r="Y94" s="13"/>
-      <c r="Z94" s="13"/>
-      <c r="AA94" s="13"/>
-      <c r="AB94" s="13"/>
-      <c r="AC94" s="13"/>
-      <c r="AD94" s="13"/>
-      <c r="AE94" s="13"/>
-      <c r="AF94" s="13"/>
-      <c r="AG94" s="13"/>
-      <c r="AH94" s="13"/>
-      <c r="AI94" s="13"/>
-      <c r="AJ94" s="13"/>
-      <c r="AK94" s="13"/>
-      <c r="AL94" s="13"/>
-      <c r="AM94" s="13"/>
-      <c r="AN94" s="13"/>
-      <c r="AO94" s="13"/>
-      <c r="AP94" s="13"/>
-      <c r="AQ94" s="13"/>
-      <c r="AR94" s="13"/>
-      <c r="AS94" s="13"/>
-      <c r="AT94" s="13"/>
-      <c r="AU94" s="13"/>
-      <c r="AV94" s="13"/>
-      <c r="AW94" s="13"/>
-      <c r="AX94" s="13"/>
-      <c r="AY94" s="13"/>
-      <c r="AZ94" s="13"/>
-      <c r="BA94" s="13"/>
-      <c r="BB94" s="13"/>
-      <c r="BC94" s="13"/>
-      <c r="BD94" s="13"/>
-      <c r="BE94" s="13"/>
-      <c r="BF94" s="13"/>
-      <c r="BG94" s="13"/>
-      <c r="BH94" s="13"/>
-      <c r="BI94" s="13"/>
-      <c r="BJ94" s="13"/>
-      <c r="BK94" s="13"/>
-      <c r="BL94" s="13"/>
-      <c r="BM94" s="13"/>
-    </row>
-    <row r="95" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="97" t="s">
+      <c r="B95" s="96"/>
+      <c r="C95" s="96"/>
+      <c r="D95" s="96"/>
+      <c r="E95" s="96"/>
+      <c r="F95" s="96"/>
+      <c r="G95" s="96"/>
+      <c r="H95" s="96"/>
+      <c r="I95" s="96"/>
+      <c r="J95" s="96"/>
+      <c r="K95" s="96"/>
+      <c r="L95" s="96"/>
+      <c r="M95" s="96"/>
+      <c r="N95" s="96"/>
+      <c r="O95" s="96"/>
+      <c r="P95" s="13"/>
+      <c r="Q95" s="13"/>
+      <c r="R95" s="13"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="13"/>
+      <c r="U95" s="13"/>
+      <c r="V95" s="13"/>
+      <c r="W95" s="13"/>
+      <c r="X95" s="13"/>
+      <c r="Y95" s="13"/>
+      <c r="Z95" s="13"/>
+      <c r="AA95" s="13"/>
+      <c r="AB95" s="13"/>
+      <c r="AC95" s="13"/>
+      <c r="AD95" s="13"/>
+      <c r="AE95" s="13"/>
+      <c r="AF95" s="13"/>
+      <c r="AG95" s="13"/>
+      <c r="AH95" s="13"/>
+      <c r="AI95" s="13"/>
+      <c r="AJ95" s="13"/>
+      <c r="AK95" s="13"/>
+      <c r="AL95" s="13"/>
+      <c r="AM95" s="13"/>
+      <c r="AN95" s="13"/>
+      <c r="AO95" s="13"/>
+      <c r="AP95" s="13"/>
+      <c r="AQ95" s="13"/>
+      <c r="AR95" s="13"/>
+      <c r="AS95" s="13"/>
+      <c r="AT95" s="13"/>
+      <c r="AU95" s="13"/>
+      <c r="AV95" s="13"/>
+      <c r="AW95" s="13"/>
+      <c r="AX95" s="13"/>
+      <c r="AY95" s="13"/>
+      <c r="AZ95" s="13"/>
+      <c r="BA95" s="13"/>
+      <c r="BB95" s="13"/>
+      <c r="BC95" s="13"/>
+      <c r="BD95" s="13"/>
+      <c r="BE95" s="13"/>
+      <c r="BF95" s="13"/>
+      <c r="BG95" s="13"/>
+      <c r="BH95" s="13"/>
+      <c r="BI95" s="13"/>
+      <c r="BJ95" s="13"/>
+      <c r="BK95" s="13"/>
+      <c r="BL95" s="13"/>
+      <c r="BM95" s="13"/>
+    </row>
+    <row r="96" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B95" s="98"/>
-      <c r="C95" s="98"/>
-      <c r="D95" s="98"/>
-      <c r="E95" s="98"/>
-      <c r="F95" s="98"/>
-      <c r="G95" s="98"/>
-      <c r="H95" s="98"/>
-      <c r="I95" s="98"/>
-      <c r="J95" s="98"/>
-      <c r="K95" s="98"/>
-      <c r="L95" s="98"/>
-      <c r="M95" s="98"/>
-      <c r="N95" s="98"/>
-      <c r="O95" s="98"/>
-    </row>
-    <row r="96" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A96" s="44">
+      <c r="B96" s="99"/>
+      <c r="C96" s="99"/>
+      <c r="D96" s="99"/>
+      <c r="E96" s="99"/>
+      <c r="F96" s="99"/>
+      <c r="G96" s="99"/>
+      <c r="H96" s="99"/>
+      <c r="I96" s="99"/>
+      <c r="J96" s="99"/>
+      <c r="K96" s="99"/>
+      <c r="L96" s="99"/>
+      <c r="M96" s="99"/>
+      <c r="N96" s="99"/>
+      <c r="O96" s="99"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" s="44">
         <v>146</v>
-      </c>
-      <c r="B96" s="57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C96" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D96" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E96" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="F96" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G96" s="44">
-        <v>403</v>
-      </c>
-      <c r="H96" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="I96" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J96" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K96" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L96" s="4">
-        <v>1016</v>
-      </c>
-      <c r="M96" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N96" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O96" s="45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="63" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
-        <v>102</v>
       </c>
       <c r="B97" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C97" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D97" s="4" t="s">
+      <c r="C97" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E97" s="4" t="s">
+      <c r="E97" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F97" s="4" t="s">
+      <c r="F97" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="G97" s="16">
-        <v>401</v>
-      </c>
-      <c r="H97" s="35" t="s">
+      <c r="G97" s="44">
+        <v>403</v>
+      </c>
+      <c r="H97" s="44" t="s">
         <v>38</v>
       </c>
       <c r="I97" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J97" s="4" t="s">
+      <c r="J97" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="K97" s="4" t="s">
+      <c r="K97" s="44" t="s">
         <v>41</v>
       </c>
       <c r="L97" s="4">
-        <v>1012</v>
-      </c>
-      <c r="M97" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="N97" s="23" t="s">
+        <v>1016</v>
+      </c>
+      <c r="M97" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N97" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O97" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="O97" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>36</v>
@@ -27684,30 +27693,30 @@
         <v>41</v>
       </c>
       <c r="L98" s="4">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M98" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N98" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O98" s="29" t="s">
+      <c r="O98" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B99" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D99" s="4">
-        <v>301</v>
+        <v>45</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>37</v>
@@ -27716,7 +27725,7 @@
         <v>37</v>
       </c>
       <c r="G99" s="16">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H99" s="35" t="s">
         <v>38</v>
@@ -27728,30 +27737,30 @@
         <v>40</v>
       </c>
       <c r="K99" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L99" s="5">
-        <v>1003</v>
-      </c>
-      <c r="M99" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="N99" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O99" s="22" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="L99" s="4">
+        <v>1013</v>
+      </c>
+      <c r="M99" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N99" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O99" s="29" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="100" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B100" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>50</v>
+      <c r="C100" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D100" s="4">
         <v>301</v>
@@ -27763,7 +27772,7 @@
         <v>37</v>
       </c>
       <c r="G100" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H100" s="35" t="s">
         <v>38</v>
@@ -27775,13 +27784,13 @@
         <v>40</v>
       </c>
       <c r="K100" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L100" s="5">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="M100" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N100" s="22" t="s">
         <v>42</v>
@@ -27792,16 +27801,16 @@
     </row>
     <row r="101" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B101" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="D101" s="4">
+        <v>301</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>37</v>
@@ -27810,7 +27819,7 @@
         <v>37</v>
       </c>
       <c r="G101" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H101" s="35" t="s">
         <v>38</v>
@@ -27825,38 +27834,38 @@
         <v>51</v>
       </c>
       <c r="L101" s="5">
-        <v>1015</v>
+        <v>1004</v>
       </c>
       <c r="M101" s="22" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="N101" s="22" t="s">
         <v>42</v>
       </c>
       <c r="O101" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B102" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C102" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D102" s="54">
-        <v>302</v>
-      </c>
-      <c r="E102" s="54" t="s">
+      <c r="C102" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E102" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F102" s="54" t="s">
+      <c r="F102" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G102" s="4">
+      <c r="G102" s="16">
         <v>403</v>
       </c>
       <c r="H102" s="35" t="s">
@@ -27865,45 +27874,45 @@
       <c r="I102" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J102" s="54" t="s">
+      <c r="J102" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K102" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L102" s="54">
-        <v>1006</v>
+      <c r="L102" s="5">
+        <v>1015</v>
       </c>
       <c r="M102" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N102" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O102" s="55" t="s">
-        <v>58</v>
+      <c r="O102" s="22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B103" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D103" s="4">
+      <c r="C103" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D103" s="54">
         <v>302</v>
       </c>
-      <c r="E103" s="4" t="s">
+      <c r="E103" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F103" s="4" t="s">
+      <c r="F103" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G103" s="16">
+      <c r="G103" s="4">
         <v>403</v>
       </c>
       <c r="H103" s="35" t="s">
@@ -27912,34 +27921,34 @@
       <c r="I103" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J103" s="4" t="s">
+      <c r="J103" s="54" t="s">
         <v>40</v>
       </c>
       <c r="K103" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L103" s="5">
-        <v>1007</v>
+        <v>51</v>
+      </c>
+      <c r="L103" s="54">
+        <v>1006</v>
       </c>
       <c r="M103" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N103" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O103" s="22" t="s">
+      <c r="O103" s="55" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B104" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D104" s="4">
         <v>302</v>
@@ -27966,10 +27975,10 @@
         <v>47</v>
       </c>
       <c r="L104" s="5">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M104" s="22" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
       <c r="N104" s="22" t="s">
         <v>42</v>
@@ -27978,15 +27987,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B105" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>173</v>
+        <v>61</v>
       </c>
       <c r="D105" s="4">
         <v>302</v>
@@ -28013,10 +28022,10 @@
         <v>47</v>
       </c>
       <c r="L105" s="5">
-        <v>5001</v>
+        <v>1008</v>
       </c>
       <c r="M105" s="22" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="N105" s="22" t="s">
         <v>42</v>
@@ -28025,15 +28034,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="31.5" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B106" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D106" s="4">
         <v>302</v>
@@ -28057,77 +28066,77 @@
         <v>40</v>
       </c>
       <c r="K106" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L106" s="5">
-        <v>1011</v>
+        <v>5001</v>
       </c>
       <c r="M106" s="22" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="N106" s="22" t="s">
         <v>42</v>
       </c>
       <c r="O106" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" ht="31.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" ht="31.5" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B107" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C107" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D107" s="16">
-        <v>305</v>
-      </c>
-      <c r="E107" s="16" t="s">
+      <c r="C107" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D107" s="4">
+        <v>302</v>
+      </c>
+      <c r="E107" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F107" s="16" t="s">
+      <c r="F107" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G107" s="26">
-        <v>400</v>
-      </c>
-      <c r="H107" s="4" t="s">
+      <c r="G107" s="16">
+        <v>403</v>
+      </c>
+      <c r="H107" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I107" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J107" s="16" t="s">
+      <c r="J107" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K107" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L107" s="17">
-        <v>1009</v>
-      </c>
-      <c r="M107" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="N107" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="O107" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" ht="63" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K107" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L107" s="5">
+        <v>1011</v>
+      </c>
+      <c r="M107" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="N107" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="O107" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="31.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="B108" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>177</v>
+        <v>72</v>
       </c>
       <c r="D108" s="16">
         <v>305</v>
@@ -28153,31 +28162,31 @@
       <c r="K108" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="L108" s="5">
-        <v>3002</v>
+      <c r="L108" s="17">
+        <v>1009</v>
       </c>
       <c r="M108" s="23" t="s">
-        <v>178</v>
+        <v>73</v>
       </c>
       <c r="N108" s="23" t="s">
         <v>176</v>
       </c>
       <c r="O108" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" ht="47.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="63" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B109" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>36</v>
+        <v>177</v>
+      </c>
+      <c r="D109" s="16">
+        <v>305</v>
       </c>
       <c r="E109" s="16" t="s">
         <v>37</v>
@@ -28200,35 +28209,65 @@
       <c r="K109" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="L109" s="18">
-        <v>3003</v>
+      <c r="L109" s="5">
+        <v>3002</v>
       </c>
       <c r="M109" s="23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="N109" s="23" t="s">
         <v>176</v>
       </c>
       <c r="O109" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" ht="47.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <v>113</v>
+      </c>
+      <c r="B110" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F110" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G110" s="26">
+        <v>400</v>
+      </c>
+      <c r="H110" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I110" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J110" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K110" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L110" s="18">
+        <v>3003</v>
+      </c>
+      <c r="M110" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="N110" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="O110" s="23" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="12"/>
-      <c r="B110" s="13"/>
-      <c r="C110" s="52"/>
-      <c r="D110" s="12"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
-      <c r="G110" s="27"/>
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="12"/>
-      <c r="K110" s="12"/>
-      <c r="L110" s="12"/>
-      <c r="M110" s="13"/>
-      <c r="N110" s="13"/>
-      <c r="O110" s="13"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
@@ -32160,6 +32199,7 @@
     <row r="342" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A342" s="12"/>
       <c r="B342" s="13"/>
+      <c r="C342" s="52"/>
       <c r="D342" s="12"/>
       <c r="E342" s="12"/>
       <c r="F342" s="12"/>
@@ -32173,29 +32213,45 @@
       <c r="N342" s="13"/>
       <c r="O342" s="13"/>
     </row>
+    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A343" s="12"/>
+      <c r="B343" s="13"/>
+      <c r="D343" s="12"/>
+      <c r="E343" s="12"/>
+      <c r="F343" s="12"/>
+      <c r="G343" s="27"/>
+      <c r="H343" s="27"/>
+      <c r="I343" s="27"/>
+      <c r="J343" s="12"/>
+      <c r="K343" s="12"/>
+      <c r="L343" s="12"/>
+      <c r="M343" s="13"/>
+      <c r="N343" s="13"/>
+      <c r="O343" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A95:O95"/>
+    <mergeCell ref="A96:O96"/>
+    <mergeCell ref="A78:O78"/>
+    <mergeCell ref="A64:O64"/>
+    <mergeCell ref="A79:O79"/>
     <mergeCell ref="A63:O63"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A19:O19"/>
     <mergeCell ref="A48:O48"/>
     <mergeCell ref="A49:O49"/>
-    <mergeCell ref="A94:O94"/>
-    <mergeCell ref="A95:O95"/>
-    <mergeCell ref="A78:O78"/>
-    <mergeCell ref="A64:O64"/>
-    <mergeCell ref="A79:O79"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L58:L62 L11:L15 L73:L77 L23:L24 L31:L32 L17:L18 L7:L9 L69:L71 L54:L56 L26:L29 L87:L90 L93 L83:L85 L99:L101 L103:L108" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L58:L62 L11:L15 L73:L77 L23:L24 L31:L32 L17:L18 L7:L9 L69:L71 L54:L56 L26:L29 L87:L90 L104:L109 L83:L85 L100:L102 L93" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K58:K62 K73:K77 K69:K71 K7:K9 K54:K56 K11:K18 K87:K93 K83:K85 K103:K109 K99:K101 K23:K45" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K58:K62 K73:K77 K69:K71 K7:K9 K54:K56 K11:K18 K23:K45 K83:K85 K104:K110 K100:K102 K87:K94" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
       <formula1>"Field,Cross Field,Cross Form"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J58:J62 J73:J77 J69:J71 J7:J9 J54:J56 J11:J18 J87:J93 J83:J85 J103:J109 J99:J101 J23:J45" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J58:J62 J73:J77 J69:J71 J7:J9 J54:J56 J11:J18 J23:J45 J83:J85 J104:J110 J100:J102 J87:J94" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
       <formula1>"Error,Warning"</formula1>
     </dataValidation>
   </dataValidations>
@@ -32205,6 +32261,67 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l29cd52af9b640b690e3347aa75f97a9>
+    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ade64af1c6a24cfdbe8da7f962b31d74>
+    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
+        </TermInfo>
+      </Terms>
+    </e62af2f156934d1aab35222180c5fbb1>
+    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
+        </TermInfo>
+      </Terms>
+    </nb82aa7489a64919aab5fd247ffa0d1e>
+    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
+        </TermInfo>
+      </Terms>
+    </f62107d924a7469492625f91956e46a6>
+    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e9be08524f454d8b979862330e952271>
+    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Value>97</Value>
+      <Value>45</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <UserInfo>
+        <DisplayName>Hunt, Martin</DisplayName>
+        <AccountId>118</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Word document" ma:contentTypeID="0x010100852E11B2A94E4937B655CB4FCD918453006DFD5C59A7CB45AAB5046F3899BB7DEC00F397826DF95DEB4B8DB89BEACF2240F1" ma:contentTypeVersion="79" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2efa76ee5d5cd602cc18ca32df57176e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9394a98c30c487d0596bd1768260a67a" ns2:_="">
     <xsd:import namespace="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
@@ -32424,68 +32541,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l29cd52af9b640b690e3347aa75f97a9>
-    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ade64af1c6a24cfdbe8da7f962b31d74>
-    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
-        </TermInfo>
-      </Terms>
-    </e62af2f156934d1aab35222180c5fbb1>
-    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
-        </TermInfo>
-      </Terms>
-    </nb82aa7489a64919aab5fd247ffa0d1e>
-    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
-        </TermInfo>
-      </Terms>
-    </f62107d924a7469492625f91956e46a6>
-    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e9be08524f454d8b979862330e952271>
-    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Value>97</Value>
-      <Value>45</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <UserInfo>
-        <DisplayName>Hunt, Martin</DisplayName>
-        <AccountId>118</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8031746-25E9-4E51-ABEB-14F1D0CC1382}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32501,22 +32575,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>